<commit_message>
Auto Loan Underwriter code commit
User ID: Sankar
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="23256" windowHeight="12540" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -17,15 +17,16 @@
     <sheet name="DMRCR_AplicationDetailsTestData" sheetId="9" r:id="rId8"/>
     <sheet name="DMRCR_FacilityInfoTestData" sheetId="10" r:id="rId9"/>
     <sheet name="DMRCR_MarginMoneyTestData" sheetId="12" r:id="rId10"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId11"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId12"/>
+    <sheet name="AL_Underwriter_L1" sheetId="14" r:id="rId11"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId12"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="352">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -900,9 +901,6 @@
     <t>Ds01_AT_AD_AL_DMC_02</t>
   </si>
   <si>
-    <t>5235</t>
-  </si>
-  <si>
     <t>own_contribution_amount</t>
   </si>
   <si>
@@ -979,14 +977,118 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>DataSet ID</t>
+  </si>
+  <si>
+    <t>Ref No</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Decision2</t>
+  </si>
+  <si>
+    <t>Note_Code</t>
+  </si>
+  <si>
+    <t>Sequence_Number</t>
+  </si>
+  <si>
+    <t>Note_Sub_Code</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>AT_AL_UNWL1_01</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_UNWL1_01</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>AT_AL_UNWL1_02</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_UNWL1_02</t>
+  </si>
+  <si>
+    <t>AT_AL_UNWL1_03</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_UNWL1_03</t>
+  </si>
+  <si>
+    <t>Recommeded</t>
+  </si>
+  <si>
+    <t>Decline</t>
+  </si>
+  <si>
+    <t>AT_AL_UNWL1_04</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_UNWL1_04</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>AT_AL_UNWL1_05</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_UNWL1_05</t>
+  </si>
+  <si>
+    <t>UserReturn</t>
+  </si>
+  <si>
+    <t>Return the Record</t>
+  </si>
+  <si>
+    <t>userType10</t>
+  </si>
+  <si>
+    <t>0308</t>
+  </si>
+  <si>
+    <t>Auto Loan -- App Data Entry</t>
+  </si>
+  <si>
+    <t>userType11</t>
+  </si>
+  <si>
+    <t>01069</t>
+  </si>
+  <si>
+    <t>Auto Loan -- Underwriter(L1)</t>
+  </si>
+  <si>
+    <t>0374</t>
+  </si>
+  <si>
+    <t>Ref_command</t>
+  </si>
+  <si>
+    <t>Return</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1021,8 +1123,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1086,6 +1195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,7 +1302,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1230,6 +1345,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
@@ -1526,83 +1662,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
-    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="38" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="38" t="s">
+      <c r="B2" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="C2" s="39" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="38" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="38" t="s">
+      <c r="B3" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B4" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="38" t="s">
-        <v>311</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C5" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>316</v>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7" s="48"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1610,6 +1791,9 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1623,16 +1807,16 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
-    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1643,13 +1827,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>294</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>29</v>
@@ -1660,29 +1844,29 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>296</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>297</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>118</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>301</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -1704,378 +1888,166 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="1" max="1" width="25.77734375" style="45" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="29"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C25" s="29"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="25" t="s">
-        <v>296</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>24</v>
-      </c>
+    <row r="1" spans="1:10">
+      <c r="A1" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" s="43">
+        <v>3656</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" s="43">
+        <v>3656</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="43">
+        <v>3656</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="43">
+        <v>3656</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="43">
+        <v>3656</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2084,21 +2056,467 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.44140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="42" t="s">
+        <v>351</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="29"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B36" s="36"/>
+      <c r="C36" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2231,40 +2649,40 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
-    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="31.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -2524,7 +2942,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -2628,18 +3046,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
-    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -3016,26 +3434,26 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="28.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -3242,30 +3660,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.88671875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.33203125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.44140625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -3474,25 +3892,25 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -3716,30 +4134,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3960,13 +4378,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4060,11 +4478,11 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Auto loan - App Data entry - Application details & Financial commitments test cases Committed.....
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -17,16 +17,18 @@
     <sheet name="DMRCR_AplicationDetailsTestData" sheetId="9" r:id="rId8"/>
     <sheet name="DMRCR_FacilityInfoTestData" sheetId="10" r:id="rId9"/>
     <sheet name="DMRCR_MarginMoneyTestData" sheetId="12" r:id="rId10"/>
-    <sheet name="AL_Underwriter_L1" sheetId="14" r:id="rId11"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId12"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId13"/>
+    <sheet name="AL_AppData_AppDetails" sheetId="15" r:id="rId11"/>
+    <sheet name="AL_AppData_CustomerDebt" sheetId="16" r:id="rId12"/>
+    <sheet name="AL_Underwriter_L1" sheetId="14" r:id="rId13"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId14"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="475">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1057,18 +1059,12 @@
     <t>Return the Record</t>
   </si>
   <si>
-    <t>userType10</t>
-  </si>
-  <si>
     <t>0308</t>
   </si>
   <si>
     <t>Auto Loan -- App Data Entry</t>
   </si>
   <si>
-    <t>userType11</t>
-  </si>
-  <si>
     <t>01069</t>
   </si>
   <si>
@@ -1082,6 +1078,381 @@
   </si>
   <si>
     <t>Return</t>
+  </si>
+  <si>
+    <t>userType05</t>
+  </si>
+  <si>
+    <t>userType06</t>
+  </si>
+  <si>
+    <t>Customer_Type</t>
+  </si>
+  <si>
+    <t>Customer_Name</t>
+  </si>
+  <si>
+    <t>ID_Type</t>
+  </si>
+  <si>
+    <t>ID_Number</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Sub_Product</t>
+  </si>
+  <si>
+    <t>Finance_Amt</t>
+  </si>
+  <si>
+    <t>Monthly_Income</t>
+  </si>
+  <si>
+    <t>Sourcing_Channel</t>
+  </si>
+  <si>
+    <t>Business_Code</t>
+  </si>
+  <si>
+    <t>Servicing_Type</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Servicing_Branch</t>
+  </si>
+  <si>
+    <t>Closing_Staff</t>
+  </si>
+  <si>
+    <t>Sourcing_Type</t>
+  </si>
+  <si>
+    <t>Sourcing_Office</t>
+  </si>
+  <si>
+    <t>Sourcing_Entity</t>
+  </si>
+  <si>
+    <t>Sourcing_Staff</t>
+  </si>
+  <si>
+    <t>Record_ID</t>
+  </si>
+  <si>
+    <t>Matching_Value</t>
+  </si>
+  <si>
+    <t>Mismatched_Value</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_01</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_01</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>8956748511</t>
+  </si>
+  <si>
+    <t>11-May-1996</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_02</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_02</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>335895644</t>
+  </si>
+  <si>
+    <t>28-Nov-1991</t>
+  </si>
+  <si>
+    <t>85000</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Azentio</t>
+  </si>
+  <si>
+    <t>Azentio Main Branch</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_03</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_03</t>
+  </si>
+  <si>
+    <t>Anbu</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>01-Feb-1985</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_04</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_04</t>
+  </si>
+  <si>
+    <t>Arivu</t>
+  </si>
+  <si>
+    <t>98765432111</t>
+  </si>
+  <si>
+    <t>01-Apr-1985</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_05</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_05</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>8654711265</t>
+  </si>
+  <si>
+    <t>19-Apr-1998</t>
+  </si>
+  <si>
+    <t>1145500</t>
+  </si>
+  <si>
+    <t>38000</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_06</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_06</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_07</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_07</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_08</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_08</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_09</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_09</t>
+  </si>
+  <si>
+    <t>4138</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_10</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_10</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_11</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_11</t>
+  </si>
+  <si>
+    <t>Pondicherry</t>
+  </si>
+  <si>
+    <t>AT_AL_APP_12</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_APP_12</t>
+  </si>
+  <si>
+    <t>Finance Type</t>
+  </si>
+  <si>
+    <t>Financial Institution</t>
+  </si>
+  <si>
+    <t>Account Nbr</t>
+  </si>
+  <si>
+    <t>Sanction Amt</t>
+  </si>
+  <si>
+    <t>Tenure(Months)</t>
+  </si>
+  <si>
+    <t>Installment Amt</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Remaining Tenure</t>
+  </si>
+  <si>
+    <t>Invalid_data</t>
+  </si>
+  <si>
+    <t>Interest_Rate</t>
+  </si>
+  <si>
+    <t>Current_Principal</t>
+  </si>
+  <si>
+    <t>Amt_Consider</t>
+  </si>
+  <si>
+    <t>Collateral_Type</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>last_Payment_Amt</t>
+  </si>
+  <si>
+    <t>Matched Currency</t>
+  </si>
+  <si>
+    <t>Mismatched Currency</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_01</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_02</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_02</t>
+  </si>
+  <si>
+    <t>Home Loan</t>
+  </si>
+  <si>
+    <t>Arab National Bank</t>
+  </si>
+  <si>
+    <t>78659984421</t>
+  </si>
+  <si>
+    <t>1030000</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>5200</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_03</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_03</t>
+  </si>
+  <si>
+    <t>3356897745</t>
+  </si>
+  <si>
+    <t>1458800</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_04</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_04</t>
+  </si>
+  <si>
+    <t>98655521022</t>
+  </si>
+  <si>
+    <t>7300</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_05</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_05</t>
+  </si>
+  <si>
+    <t>3300</t>
+  </si>
+  <si>
+    <t>@#</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_06</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_06</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_07</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_07</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_08</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_08</t>
+  </si>
+  <si>
+    <t>AT_AL_CUD_09</t>
+  </si>
+  <si>
+    <t>DS_AT_AL_CUD_09</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1673,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1366,6 +1737,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
@@ -1664,7 +2038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
@@ -1686,7 +2062,7 @@
         <v>303</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1756,34 +2132,34 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>343</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>344</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="38" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -1888,10 +2264,1051 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y13"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" style="45" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" customWidth="1"/>
+    <col min="20" max="20" width="19.5546875" customWidth="1"/>
+    <col min="21" max="21" width="16.5546875" customWidth="1"/>
+    <col min="22" max="22" width="13.77734375" customWidth="1"/>
+    <col min="23" max="23" width="10.21875" customWidth="1"/>
+    <col min="24" max="24" width="15" customWidth="1"/>
+    <col min="25" max="25" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>360</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>361</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>364</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>365</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1" s="40" t="s">
+        <v>367</v>
+      </c>
+      <c r="U1" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="V1" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="W1" s="40" t="s">
+        <v>370</v>
+      </c>
+      <c r="X1" s="41" t="s">
+        <v>371</v>
+      </c>
+      <c r="Y1" s="41" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>377</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>380</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>381</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>382</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="49" t="s">
+        <v>383</v>
+      </c>
+      <c r="M3" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="N3" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="S3" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="T3" s="49" t="s">
+        <v>387</v>
+      </c>
+      <c r="U3" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="V3" s="49" t="s">
+        <v>388</v>
+      </c>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>391</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>392</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>393</v>
+      </c>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>397</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>402</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>403</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>404</v>
+      </c>
+      <c r="L6" s="49" t="s">
+        <v>405</v>
+      </c>
+      <c r="M6" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="O6" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="P6" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q6" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="C7" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C8" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49" t="s">
+        <v>404</v>
+      </c>
+      <c r="L8" s="49" t="s">
+        <v>405</v>
+      </c>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49" t="s">
+        <v>414</v>
+      </c>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="C11" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49" t="s">
+        <v>414</v>
+      </c>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C12" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49" t="s">
+        <v>385</v>
+      </c>
+      <c r="Y12" s="49" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="C13" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>422</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>423</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>424</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>426</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>427</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>428</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>429</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>430</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>431</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>432</v>
+      </c>
+      <c r="O1" s="41" t="s">
+        <v>433</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q1" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="R1" s="41" t="s">
+        <v>436</v>
+      </c>
+      <c r="S1" s="41" t="s">
+        <v>437</v>
+      </c>
+      <c r="T1" s="41" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="C3" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>443</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>444</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>445</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>446</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>447</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>448</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>449</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>450</v>
+      </c>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>444</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>454</v>
+      </c>
+      <c r="H4" s="43">
+        <v>72</v>
+      </c>
+      <c r="I4" s="43">
+        <v>6800</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>449</v>
+      </c>
+      <c r="K4" s="43">
+        <v>71</v>
+      </c>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43">
+        <v>12</v>
+      </c>
+      <c r="N4" s="43">
+        <v>3500</v>
+      </c>
+      <c r="O4" s="43">
+        <v>50000</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>456</v>
+      </c>
+      <c r="R4" s="43">
+        <v>6800</v>
+      </c>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="C5" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>444</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="43">
+        <v>72</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C6" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44" t="s">
+        <v>464</v>
+      </c>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="C7" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="C8" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44" t="s">
+        <v>449</v>
+      </c>
+      <c r="T8" s="44" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="C9" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="C10" s="43">
+        <v>5256</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2054,12 +3471,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2297,66 +3714,66 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="42" t="s">
-        <v>327</v>
+      <c r="A20" s="22" t="s">
+        <v>373</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>328</v>
+        <v>374</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="42" t="s">
-        <v>330</v>
+      <c r="A21" s="22" t="s">
+        <v>378</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>331</v>
+        <v>379</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="42" t="s">
-        <v>332</v>
+      <c r="A22" s="22" t="s">
+        <v>389</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>333</v>
+        <v>390</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="42" t="s">
-        <v>336</v>
+      <c r="A23" s="22" t="s">
+        <v>394</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>337</v>
+        <v>395</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="42" t="s">
-        <v>351</v>
+      <c r="A24" s="22" t="s">
+        <v>399</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>337</v>
+        <v>400</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="42" t="s">
-        <v>339</v>
+      <c r="A25" s="22" t="s">
+        <v>406</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>340</v>
+        <v>407</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>24</v>
@@ -2364,10 +3781,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>264</v>
+        <v>408</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>409</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>24</v>
@@ -2375,10 +3792,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>266</v>
+        <v>410</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>411</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>24</v>
@@ -2386,10 +3803,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>269</v>
+        <v>412</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>413</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>24</v>
@@ -2397,101 +3814,332 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="29"/>
+        <v>415</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C30" s="29" t="s">
+      <c r="A30" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C31" s="29"/>
+      <c r="A31" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34" t="s">
+      <c r="A32" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="C33" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C34" s="35" t="s">
+        <v>451</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="22" t="s">
+        <v>462</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="42" t="s">
+        <v>349</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="29"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C52" s="29"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C35" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="24" t="s">
+      <c r="C56" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="25" t="s">
+      <c r="B57" s="36"/>
+      <c r="C57" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B58" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="C37" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
+      <c r="C58" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C59" s="35" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2500,7 +4148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Login code and under writer edited code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="477">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1453,12 +1453,19 @@
   </si>
   <si>
     <t>DS_AT_AL_CUD_09</t>
+  </si>
+  <si>
+    <t>5295</t>
+  </si>
+  <si>
+    <t>5256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2044,11 +2051,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="19.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.88671875" collapsed="true"/>
+    <col min="5" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2122,7 +2129,9 @@
       <c r="A6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>311</v>
+      </c>
       <c r="C6" s="39" t="s">
         <v>306</v>
       </c>
@@ -2185,14 +2194,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.44140625" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2272,31 +2281,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" style="45" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" customWidth="1"/>
-    <col min="20" max="20" width="19.5546875" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" customWidth="1"/>
-    <col min="22" max="22" width="13.77734375" customWidth="1"/>
-    <col min="23" max="23" width="10.21875" customWidth="1"/>
-    <col min="24" max="24" width="15" customWidth="1"/>
-    <col min="25" max="25" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="45" width="8.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="11.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.34375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -2770,7 +2779,7 @@
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49" t="s">
-        <v>414</v>
+        <v>476</v>
       </c>
       <c r="X10" s="49"/>
       <c r="Y10" s="49"/>
@@ -2895,25 +2904,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
-    <col min="20" max="20" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -3313,15 +3322,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="45" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="45" width="25.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="4" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3481,14 +3490,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4158,13 +4167,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4299,38 +4308,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="35.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="40.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="32.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="43.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="32.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="30.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="28.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="4" width="32.109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="21.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="39.6640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="15.5546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="40.88671875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="4" width="31.109375" collapsed="true"/>
+    <col min="21" max="23" customWidth="true" style="4" width="31.33203125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.6640625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="4" width="19.44140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="20.6640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="31.44140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="4" width="26.6640625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="19.5546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="4" width="26.44140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="4" width="17.5546875" collapsed="true"/>
+    <col min="34" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -4590,7 +4599,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>316</v>
+        <v>475</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -4696,16 +4705,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="24.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="24.5546875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="4" width="29.6640625" collapsed="true"/>
+    <col min="7" max="45" customWidth="true" style="4" width="41.44140625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.88671875" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="23.88671875" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="16.5546875" collapsed="true"/>
+    <col min="49" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -5084,24 +5093,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="39.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="40.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="29.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="23.88671875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="4" width="39.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="20.44140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="18.5546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="19" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5310,28 +5319,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.88671875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.109375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.44140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="43.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="38.109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="31.44140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -5542,23 +5551,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5784,28 +5793,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6028,11 +6037,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6128,9 +6137,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Updated test data committed for auto loan application details
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="23256" windowHeight="12540" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="475">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -978,9 +978,6 @@
     <t>Auto Loan DIsChkr</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>TestCaseID</t>
   </si>
   <si>
@@ -1270,9 +1267,6 @@
   </si>
   <si>
     <t>DS_AT_AL_APP_09</t>
-  </si>
-  <si>
-    <t>4138</t>
   </si>
   <si>
     <t>AT_AL_APP_10</t>
@@ -1465,7 +1459,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2049,13 +2042,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="15.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.88671875" collapsed="true"/>
-    <col min="5" max="16384" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2069,7 +2062,7 @@
         <v>303</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2127,7 +2120,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>311</v>
@@ -2136,39 +2129,39 @@
         <v>306</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="38" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D8" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>346</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2192,16 +2185,16 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.44140625" collapsed="true"/>
-    <col min="8" max="16384" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2275,122 +2268,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="45" width="8.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="13.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="11.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.34375" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" style="45" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>319</v>
-      </c>
       <c r="D1" s="40" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>353</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>354</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>355</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>356</v>
       </c>
       <c r="I1" s="40" t="s">
         <v>100</v>
       </c>
       <c r="J1" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="K1" s="40" t="s">
         <v>357</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>358</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>359</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="N1" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="O1" s="40" t="s">
         <v>361</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>362</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="R1" s="40" t="s">
         <v>364</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="S1" s="40" t="s">
         <v>365</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="T1" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="U1" s="40" t="s">
         <v>367</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="V1" s="40" t="s">
         <v>368</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="W1" s="40" t="s">
         <v>369</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="X1" s="41" t="s">
         <v>370</v>
       </c>
-      <c r="X1" s="41" t="s">
+      <c r="Y1" s="41" t="s">
         <v>371</v>
-      </c>
-      <c r="Y1" s="41" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>373</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>374</v>
       </c>
       <c r="C2" s="43">
         <v>5256</v>
@@ -2399,16 +2392,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>376</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>377</v>
       </c>
       <c r="I2" s="49"/>
       <c r="J2" s="49"/>
@@ -2430,10 +2423,10 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>378</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>379</v>
       </c>
       <c r="C3" s="43">
         <v>5256</v>
@@ -2442,16 +2435,16 @@
         <v>7</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="49" t="s">
+        <v>380</v>
+      </c>
+      <c r="H3" s="49" t="s">
         <v>381</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>382</v>
       </c>
       <c r="I3" s="49" t="s">
         <v>109</v>
@@ -2463,10 +2456,10 @@
         <v>117</v>
       </c>
       <c r="L3" s="49" t="s">
+        <v>382</v>
+      </c>
+      <c r="M3" s="49" t="s">
         <v>383</v>
-      </c>
-      <c r="M3" s="49" t="s">
-        <v>384</v>
       </c>
       <c r="N3" s="49" t="s">
         <v>159</v>
@@ -2478,22 +2471,22 @@
         <v>161</v>
       </c>
       <c r="Q3" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="R3" s="49" t="s">
         <v>385</v>
-      </c>
-      <c r="R3" s="49" t="s">
-        <v>386</v>
       </c>
       <c r="S3" s="49" t="s">
         <v>160</v>
       </c>
       <c r="T3" s="49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="U3" s="49" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="49" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W3" s="49"/>
       <c r="X3" s="49"/>
@@ -2501,10 +2494,10 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>389</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>390</v>
       </c>
       <c r="C4" s="43">
         <v>5256</v>
@@ -2513,16 +2506,16 @@
         <v>7</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="49" t="s">
+        <v>391</v>
+      </c>
+      <c r="H4" s="49" t="s">
         <v>392</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>393</v>
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="49"/>
@@ -2544,10 +2537,10 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>394</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>395</v>
       </c>
       <c r="C5" s="43">
         <v>5256</v>
@@ -2556,16 +2549,16 @@
         <v>7</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="49" t="s">
+        <v>396</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>397</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>398</v>
       </c>
       <c r="I5" s="49"/>
       <c r="J5" s="49"/>
@@ -2587,10 +2580,10 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>399</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>400</v>
       </c>
       <c r="C6" s="43">
         <v>5256</v>
@@ -2599,16 +2592,16 @@
         <v>7</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="49" t="s">
+        <v>401</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>402</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>403</v>
       </c>
       <c r="I6" s="49" t="s">
         <v>109</v>
@@ -2617,13 +2610,13 @@
         <v>110</v>
       </c>
       <c r="K6" s="49" t="s">
+        <v>403</v>
+      </c>
+      <c r="L6" s="49" t="s">
         <v>404</v>
       </c>
-      <c r="L6" s="49" t="s">
-        <v>405</v>
-      </c>
       <c r="M6" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N6" s="49" t="s">
         <v>159</v>
@@ -2635,7 +2628,7 @@
         <v>161</v>
       </c>
       <c r="Q6" s="49" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R6" s="49"/>
       <c r="S6" s="49"/>
@@ -2648,10 +2641,10 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>406</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>407</v>
       </c>
       <c r="C7" s="43">
         <v>5256</v>
@@ -2681,10 +2674,10 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>408</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>409</v>
       </c>
       <c r="C8" s="43">
         <v>5256</v>
@@ -2697,10 +2690,10 @@
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
       <c r="K8" s="49" t="s">
+        <v>403</v>
+      </c>
+      <c r="L8" s="49" t="s">
         <v>404</v>
-      </c>
-      <c r="L8" s="49" t="s">
-        <v>405</v>
       </c>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
@@ -2718,10 +2711,10 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>410</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>411</v>
       </c>
       <c r="C9" s="43">
         <v>5256</v>
@@ -2751,10 +2744,10 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>412</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>413</v>
       </c>
       <c r="C10" s="43">
         <v>5256</v>
@@ -2779,17 +2772,17 @@
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="X10" s="49"/>
       <c r="Y10" s="49"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C11" s="43">
         <v>5256</v>
@@ -2813,18 +2806,16 @@
       <c r="T11" s="49"/>
       <c r="U11" s="49"/>
       <c r="V11" s="49"/>
-      <c r="W11" s="49" t="s">
-        <v>414</v>
-      </c>
+      <c r="W11" s="49"/>
       <c r="X11" s="49"/>
       <c r="Y11" s="49"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C12" s="43">
         <v>5256</v>
@@ -2850,18 +2841,18 @@
       <c r="V12" s="49"/>
       <c r="W12" s="49"/>
       <c r="X12" s="49" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Y12" s="49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C13" s="43">
         <v>5256</v>
@@ -2898,101 +2889,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>319</v>
-      </c>
       <c r="D1" s="41" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>421</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>422</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>423</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="H1" s="41" t="s">
         <v>424</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>426</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="K1" s="41" t="s">
         <v>427</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="L1" s="41" t="s">
         <v>428</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="M1" s="41" t="s">
         <v>429</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="N1" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="O1" s="41" t="s">
         <v>431</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="P1" s="41" t="s">
         <v>432</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="Q1" s="41" t="s">
         <v>433</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="R1" s="41" t="s">
         <v>434</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="S1" s="41" t="s">
         <v>435</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="T1" s="41" t="s">
         <v>436</v>
-      </c>
-      <c r="S1" s="41" t="s">
-        <v>437</v>
-      </c>
-      <c r="T1" s="41" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="22" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C2" s="43">
         <v>5256</v>
@@ -3017,37 +3008,37 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C3" s="43">
         <v>5256</v>
       </c>
       <c r="D3" s="44" t="s">
+        <v>441</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>442</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>443</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="G3" s="44" t="s">
         <v>444</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="H3" s="44" t="s">
         <v>445</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="I3" s="44" t="s">
         <v>446</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="J3" s="44" t="s">
         <v>447</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="K3" s="44" t="s">
         <v>448</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>449</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>450</v>
       </c>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
@@ -3061,25 +3052,25 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="22" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C4" s="43">
         <v>5256</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H4" s="43">
         <v>72</v>
@@ -3088,7 +3079,7 @@
         <v>6800</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K4" s="43">
         <v>71</v>
@@ -3104,10 +3095,10 @@
         <v>50000</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Q4" s="43" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="R4" s="43">
         <v>6800</v>
@@ -3117,10 +3108,10 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C5" s="43">
         <v>5256</v>
@@ -3129,10 +3120,10 @@
         <v>109</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G5" s="44" t="s">
         <v>117</v>
@@ -3141,11 +3132,11 @@
         <v>72</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="44" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
@@ -3159,10 +3150,10 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="22" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C6" s="43">
         <v>5256</v>
@@ -3175,12 +3166,12 @@
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
       <c r="L6" s="44" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
@@ -3193,10 +3184,10 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="22" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C7" s="43">
         <v>5256</v>
@@ -3221,10 +3212,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="22" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C8" s="43">
         <v>5256</v>
@@ -3245,18 +3236,18 @@
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
       <c r="S8" s="44" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="T8" s="44" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C9" s="43">
         <v>5256</v>
@@ -3281,10 +3272,10 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="22" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C10" s="43">
         <v>5256</v>
@@ -3320,63 +3311,63 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="45" width="25.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="4" width="12.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>325</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>328</v>
       </c>
       <c r="C2" s="43">
         <v>3656</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
@@ -3387,10 +3378,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>330</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>331</v>
       </c>
       <c r="C3" s="43">
         <v>3656</v>
@@ -3405,10 +3396,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>332</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>333</v>
       </c>
       <c r="C4" s="43">
         <v>3656</v>
@@ -3416,13 +3407,13 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G4" s="44" t="s">
         <v>82</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I4" s="44" t="s">
         <v>93</v>
@@ -3433,19 +3424,19 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="42" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>336</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>337</v>
       </c>
       <c r="C5" s="43">
         <v>3656</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
@@ -3455,10 +3446,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>339</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>340</v>
       </c>
       <c r="C6" s="43">
         <v>3656</v>
@@ -3488,16 +3479,16 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3724,10 +3715,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>373</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>374</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>24</v>
@@ -3735,10 +3726,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>378</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>379</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>24</v>
@@ -3746,10 +3737,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>389</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>390</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>24</v>
@@ -3757,10 +3748,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>394</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>395</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>24</v>
@@ -3768,10 +3759,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>399</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>400</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>24</v>
@@ -3779,10 +3770,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="B25" s="22" t="s">
         <v>406</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>407</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>24</v>
@@ -3790,10 +3781,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>408</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>409</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>24</v>
@@ -3801,10 +3792,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>410</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>411</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>24</v>
@@ -3812,10 +3803,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>412</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>413</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>24</v>
@@ -3823,10 +3814,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>24</v>
@@ -3834,10 +3825,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>24</v>
@@ -3845,10 +3836,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>24</v>
@@ -3856,10 +3847,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="22" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>24</v>
@@ -3867,10 +3858,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>24</v>
@@ -3878,10 +3869,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="22" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>24</v>
@@ -3889,10 +3880,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>24</v>
@@ -3900,10 +3891,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="22" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>24</v>
@@ -3911,10 +3902,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="22" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>24</v>
@@ -3922,10 +3913,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="22" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>24</v>
@@ -3933,10 +3924,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>24</v>
@@ -3944,10 +3935,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="22" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>24</v>
@@ -3955,10 +3946,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>328</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>24</v>
@@ -3966,10 +3957,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>330</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>331</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>24</v>
@@ -3977,10 +3968,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" s="22" t="s">
         <v>332</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>333</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>24</v>
@@ -3988,10 +3979,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="42" t="s">
+        <v>335</v>
+      </c>
+      <c r="B44" s="22" t="s">
         <v>336</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>337</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>24</v>
@@ -3999,10 +3990,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>24</v>
@@ -4010,10 +4001,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>339</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>340</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>24</v>
@@ -4165,15 +4156,15 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4306,40 +4297,40 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="20.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="35.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="40.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="32.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="43.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="32.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="30.88671875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="28.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="4" width="32.109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="21.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="39.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="15.5546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="40.88671875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="4" width="31.109375" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="4" width="31.33203125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.6640625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="19.44140625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="20.6640625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="4" width="31.44140625" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="4" width="26.6640625" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="4" width="19.5546875" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="4" width="26.44140625" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="4" width="17.5546875" collapsed="true"/>
-    <col min="34" max="16384" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -4599,7 +4590,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -4703,18 +4694,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="24.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="24.5546875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="4" width="29.6640625" collapsed="true"/>
-    <col min="7" max="45" customWidth="true" style="4" width="41.44140625" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.88671875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="23.88671875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5546875" collapsed="true"/>
-    <col min="49" max="16384" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -5091,26 +5082,26 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="28.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="39.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="20.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="40.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="29.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.88671875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="23.88671875" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" style="4" width="39.6640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="20.44140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="18.5546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="19" max="16384" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5317,30 +5308,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="43.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.6640625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="29.33203125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="38.109375" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="36.33203125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="31.44140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -5549,25 +5540,25 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.5546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="33.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5791,30 +5782,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="22.44140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6035,13 +6026,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6135,11 +6126,11 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Data entry updated test data commited
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="475">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1056,9 +1056,6 @@
     <t>Return the Record</t>
   </si>
   <si>
-    <t>0308</t>
-  </si>
-  <si>
     <t>Auto Loan -- App Data Entry</t>
   </si>
   <si>
@@ -1449,20 +1446,19 @@
     <t>DS_AT_AL_CUD_09</t>
   </si>
   <si>
-    <t>5295</t>
-  </si>
-  <si>
     <t>5256</t>
   </si>
   <si>
-    <t>5298</t>
+    <t>5313</t>
+  </si>
+  <si>
+    <t>0354</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2043,16 +2039,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
-    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2066,7 +2062,7 @@
         <v>303</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2138,34 +2134,34 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="38" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>342</v>
+        <v>474</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>306</v>
       </c>
       <c r="D8" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2191,14 +2187,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
-    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2272,37 +2268,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="45" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="11.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" style="45" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -2316,96 +2312,96 @@
         <v>318</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>351</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>353</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>354</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>355</v>
       </c>
       <c r="I1" s="40" t="s">
         <v>100</v>
       </c>
       <c r="J1" s="40" t="s">
+        <v>355</v>
+      </c>
+      <c r="K1" s="40" t="s">
         <v>356</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>357</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>358</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="N1" s="40" t="s">
         <v>359</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="O1" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>361</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>362</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="R1" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="S1" s="40" t="s">
         <v>364</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="T1" s="40" t="s">
         <v>365</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="U1" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="V1" s="40" t="s">
         <v>367</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="W1" s="40" t="s">
         <v>368</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="X1" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="X1" s="41" t="s">
+      <c r="Y1" s="41" t="s">
         <v>370</v>
-      </c>
-      <c r="Y1" s="41" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>373</v>
-      </c>
       <c r="C2" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D2" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>375</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>376</v>
       </c>
       <c r="I2" s="49"/>
       <c r="J2" s="49"/>
@@ -2427,28 +2423,28 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>378</v>
-      </c>
       <c r="C3" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="49" t="s">
+        <v>379</v>
+      </c>
+      <c r="H3" s="49" t="s">
         <v>380</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>381</v>
       </c>
       <c r="I3" s="49" t="s">
         <v>109</v>
@@ -2460,10 +2456,10 @@
         <v>117</v>
       </c>
       <c r="L3" s="49" t="s">
+        <v>381</v>
+      </c>
+      <c r="M3" s="49" t="s">
         <v>382</v>
-      </c>
-      <c r="M3" s="49" t="s">
-        <v>383</v>
       </c>
       <c r="N3" s="49" t="s">
         <v>159</v>
@@ -2475,22 +2471,22 @@
         <v>161</v>
       </c>
       <c r="Q3" s="49" t="s">
+        <v>383</v>
+      </c>
+      <c r="R3" s="49" t="s">
         <v>384</v>
-      </c>
-      <c r="R3" s="49" t="s">
-        <v>385</v>
       </c>
       <c r="S3" s="49" t="s">
         <v>160</v>
       </c>
       <c r="T3" s="49" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="U3" s="49" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W3" s="49"/>
       <c r="X3" s="49"/>
@@ -2498,28 +2494,28 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>389</v>
-      </c>
       <c r="C4" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="49" t="s">
+        <v>390</v>
+      </c>
+      <c r="H4" s="49" t="s">
         <v>391</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>392</v>
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="49"/>
@@ -2541,28 +2537,28 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>394</v>
-      </c>
       <c r="C5" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>396</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>397</v>
       </c>
       <c r="I5" s="49"/>
       <c r="J5" s="49"/>
@@ -2584,28 +2580,28 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>398</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>399</v>
-      </c>
       <c r="C6" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="49" t="s">
+        <v>400</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>401</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>402</v>
       </c>
       <c r="I6" s="49" t="s">
         <v>109</v>
@@ -2614,13 +2610,13 @@
         <v>110</v>
       </c>
       <c r="K6" s="49" t="s">
+        <v>402</v>
+      </c>
+      <c r="L6" s="49" t="s">
         <v>403</v>
       </c>
-      <c r="L6" s="49" t="s">
-        <v>404</v>
-      </c>
       <c r="M6" s="49" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N6" s="49" t="s">
         <v>159</v>
@@ -2632,7 +2628,7 @@
         <v>161</v>
       </c>
       <c r="Q6" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R6" s="49"/>
       <c r="S6" s="49"/>
@@ -2645,13 +2641,13 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>405</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>406</v>
-      </c>
       <c r="C7" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
@@ -2678,13 +2674,13 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>408</v>
-      </c>
       <c r="C8" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -2694,10 +2690,10 @@
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
       <c r="K8" s="49" t="s">
+        <v>402</v>
+      </c>
+      <c r="L8" s="49" t="s">
         <v>403</v>
-      </c>
-      <c r="L8" s="49" t="s">
-        <v>404</v>
       </c>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
@@ -2715,13 +2711,13 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>409</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>410</v>
-      </c>
       <c r="C9" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -2748,13 +2744,13 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>412</v>
-      </c>
       <c r="C10" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -2776,20 +2772,20 @@
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="X10" s="49"/>
       <c r="Y10" s="49"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>413</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>414</v>
-      </c>
       <c r="C11" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
@@ -2816,13 +2812,13 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>416</v>
-      </c>
       <c r="C12" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -2845,21 +2841,21 @@
       <c r="V12" s="49"/>
       <c r="W12" s="49"/>
       <c r="X12" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Y12" s="49" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>419</v>
-      </c>
       <c r="C13" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -2893,31 +2889,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -2931,66 +2927,66 @@
         <v>318</v>
       </c>
       <c r="D1" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>420</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>421</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>422</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="41" t="s">
         <v>423</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>424</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="K1" s="41" t="s">
         <v>426</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="L1" s="41" t="s">
         <v>427</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="M1" s="41" t="s">
         <v>428</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="N1" s="41" t="s">
         <v>429</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="O1" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="P1" s="41" t="s">
         <v>431</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="Q1" s="41" t="s">
         <v>432</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="R1" s="41" t="s">
         <v>433</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="S1" s="41" t="s">
         <v>434</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="T1" s="41" t="s">
         <v>435</v>
-      </c>
-      <c r="T1" s="41" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>437</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>438</v>
-      </c>
       <c r="C2" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
@@ -3012,37 +3008,37 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>439</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="43">
+        <v>5308</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="43">
-        <v>5256</v>
-      </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="44" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="F3" s="44" t="s">
         <v>442</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="44" t="s">
         <v>443</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="H3" s="44" t="s">
         <v>444</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="I3" s="44" t="s">
         <v>445</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="J3" s="44" t="s">
         <v>446</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="K3" s="44" t="s">
         <v>447</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>448</v>
       </c>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
@@ -3056,25 +3052,25 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>449</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="43">
+        <v>5308</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>440</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>441</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>450</v>
       </c>
-      <c r="C4" s="43">
-        <v>5256</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>441</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>442</v>
-      </c>
-      <c r="F4" s="44" t="s">
+      <c r="G4" s="44" t="s">
         <v>451</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>452</v>
       </c>
       <c r="H4" s="43">
         <v>72</v>
@@ -3083,7 +3079,7 @@
         <v>6800</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K4" s="43">
         <v>71</v>
@@ -3099,10 +3095,10 @@
         <v>50000</v>
       </c>
       <c r="P4" s="43" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q4" s="43" t="s">
         <v>453</v>
-      </c>
-      <c r="Q4" s="43" t="s">
-        <v>454</v>
       </c>
       <c r="R4" s="43">
         <v>6800</v>
@@ -3112,22 +3108,22 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>455</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>456</v>
-      </c>
       <c r="C5" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>109</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G5" s="44" t="s">
         <v>117</v>
@@ -3136,11 +3132,11 @@
         <v>72</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="44" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
@@ -3154,13 +3150,13 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>460</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>461</v>
-      </c>
       <c r="C6" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D6" s="44" t="s">
         <v>109</v>
@@ -3170,12 +3166,12 @@
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
       <c r="L6" s="44" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
@@ -3188,13 +3184,13 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>465</v>
-      </c>
       <c r="C7" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
@@ -3216,13 +3212,13 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>466</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>467</v>
-      </c>
       <c r="C8" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
@@ -3240,21 +3236,21 @@
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
       <c r="S8" s="44" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="T8" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>470</v>
-      </c>
       <c r="C9" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="44"/>
@@ -3276,13 +3272,13 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>471</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>472</v>
-      </c>
       <c r="C10" s="43">
-        <v>5256</v>
+        <v>5308</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="44"/>
@@ -3317,15 +3313,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="45" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3485,14 +3481,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3719,10 +3715,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>372</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>373</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>24</v>
@@ -3730,10 +3726,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>377</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>378</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>24</v>
@@ -3741,10 +3737,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>388</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>389</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>24</v>
@@ -3752,10 +3748,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>393</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>394</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>24</v>
@@ -3763,10 +3759,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>398</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>399</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>24</v>
@@ -3774,10 +3770,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B25" s="22" t="s">
         <v>405</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>406</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>24</v>
@@ -3785,10 +3781,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>407</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>408</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>24</v>
@@ -3796,10 +3792,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>409</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>410</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>24</v>
@@ -3807,10 +3803,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>411</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>412</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>24</v>
@@ -3818,10 +3814,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>413</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>414</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>24</v>
@@ -3829,10 +3825,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>415</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>416</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>24</v>
@@ -3840,10 +3836,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>418</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>419</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>24</v>
@@ -3851,10 +3847,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>437</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>438</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>24</v>
@@ -3862,10 +3858,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>439</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>440</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>24</v>
@@ -3873,10 +3869,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>449</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>450</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>24</v>
@@ -3884,10 +3880,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>455</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>456</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>24</v>
@@ -3895,10 +3891,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="B36" s="22" t="s">
         <v>460</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>461</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>24</v>
@@ -3906,10 +3902,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="B37" s="22" t="s">
         <v>464</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>465</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>24</v>
@@ -3917,10 +3913,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B38" s="22" t="s">
         <v>466</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>467</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>24</v>
@@ -3928,10 +3924,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B39" s="22" t="s">
         <v>469</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>470</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>24</v>
@@ -3939,10 +3935,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="B40" s="22" t="s">
         <v>471</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>472</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>24</v>
@@ -3994,7 +3990,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>336</v>
@@ -4162,13 +4158,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4303,38 +4299,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
-    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
-    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -4594,7 +4590,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -4700,16 +4696,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
-    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
-    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
-    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -5088,24 +5084,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5314,28 +5310,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -5546,23 +5542,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5788,28 +5784,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6032,11 +6028,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6132,9 +6128,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
JSE click code changes commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="477">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1453,12 +1453,19 @@
   </si>
   <si>
     <t>0354</t>
+  </si>
+  <si>
+    <t>5315</t>
+  </si>
+  <si>
+    <t>0315</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -2044,11 +2051,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
+    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2123,7 +2130,7 @@
         <v>340</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>311</v>
+        <v>476</v>
       </c>
       <c r="C6" s="39" t="s">
         <v>306</v>
@@ -2187,14 +2194,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2274,31 +2281,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" style="45" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="45" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -2895,25 +2902,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -3313,15 +3320,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="45" width="25.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3481,14 +3488,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4158,13 +4165,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4299,38 +4306,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
+    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -4590,7 +4597,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -4696,16 +4703,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
+    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -5084,24 +5091,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5310,28 +5317,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -5542,23 +5549,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5784,28 +5791,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6028,11 +6035,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6128,9 +6135,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Auto loan code committed from arul
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="23256" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -25,15 +25,20 @@
     <sheet name="ALADEntryIdentificationDetails" sheetId="20" r:id="rId16"/>
     <sheet name="ALAppdataEntryIncomedetails" sheetId="18" r:id="rId17"/>
     <sheet name="AutoLoanCustomerSearch" sheetId="21" r:id="rId18"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId19"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId20"/>
+    <sheet name="AutoLoan_IdentificationDetails" sheetId="22" r:id="rId19"/>
+    <sheet name="AutoLoan_ReferenceDetails" sheetId="23" r:id="rId20"/>
+    <sheet name="AutoLoan_ManualBank" sheetId="24" r:id="rId21"/>
+    <sheet name="AutoLoan_CustomerDetails" sheetId="25" r:id="rId22"/>
+    <sheet name="AppDataCheck_ApplicationDetails" sheetId="26" r:id="rId23"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId24"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId25"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="746">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1908,13 +1913,379 @@
   </si>
   <si>
     <t>AT_AL_CUS_11</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_01</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_01_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_02</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_02_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_03</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_03_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_04</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_04_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_05</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_05_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_06</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_06_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_07</t>
+  </si>
+  <si>
+    <t>AT_AL_IDA_07_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_03</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_03_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_04</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_04_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_05</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_05_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_07</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_07_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_08</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_08_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_09</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_09_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_10</t>
+  </si>
+  <si>
+    <t>AT_AL_APPDATAENTRY_REFDETAILS_10_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_01</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_01_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_02</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_02_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_03</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_03_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_04</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_04_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_05</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_05_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_06</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_06_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_07</t>
+  </si>
+  <si>
+    <t>AT_AL_MB_07_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_AD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_AD_01_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_07</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_07_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_08</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_08_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_09</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_09_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_10</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_10_D1</t>
+  </si>
+  <si>
+    <t>IDType</t>
+  </si>
+  <si>
+    <t>IDNumber</t>
+  </si>
+  <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>IssuingAuthority</t>
+  </si>
+  <si>
+    <t>CountryOfIssue</t>
+  </si>
+  <si>
+    <t>5308</t>
+  </si>
+  <si>
+    <t>Government of KSA</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>#@#@#@</t>
+  </si>
+  <si>
+    <t>CPR</t>
+  </si>
+  <si>
+    <t>Government of Bahrain</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>NatureOfEmployment</t>
+  </si>
+  <si>
+    <t>CompanyType</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>ProfessionType</t>
+  </si>
+  <si>
+    <t>StatutoryAuthority</t>
+  </si>
+  <si>
+    <t>EmploymentEndDate</t>
+  </si>
+  <si>
+    <t>EmployerPhoneExtension</t>
+  </si>
+  <si>
+    <t>NoOfPartners</t>
+  </si>
+  <si>
+    <t>NatureOfBusiness</t>
+  </si>
+  <si>
+    <t>RegisteredBusinessName</t>
+  </si>
+  <si>
+    <t>RegisteredBusinessNumber</t>
+  </si>
+  <si>
+    <t>BusinessRegistrationDate</t>
+  </si>
+  <si>
+    <t>OfficePremisesType</t>
+  </si>
+  <si>
+    <t>ShareHolderPercentage</t>
+  </si>
+  <si>
+    <t>NoOfEmployees</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>Self Employed</t>
+  </si>
+  <si>
+    <t>H.U.F.</t>
+  </si>
+  <si>
+    <t>ARTIST</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Rented</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Multinational Company (MNC)</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>TEMPORARY</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>Owned</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>##$$##</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>BankCode</t>
+  </si>
+  <si>
+    <t>AccountBranch</t>
+  </si>
+  <si>
+    <t>BankAccountType</t>
+  </si>
+  <si>
+    <t>BankAccountNumber</t>
+  </si>
+  <si>
+    <t>CurrencyCode</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>testag</t>
+  </si>
+  <si>
+    <t>salem</t>
+  </si>
+  <si>
+    <t>Card Account</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>testupdate</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Current Account</t>
+  </si>
+  <si>
+    <t>$$$$</t>
+  </si>
+  <si>
+    <t>PRERNA</t>
+  </si>
+  <si>
+    <t>#$#$#$</t>
+  </si>
+  <si>
+    <t>DataSetID</t>
+  </si>
+  <si>
+    <t>userType15</t>
+  </si>
+  <si>
+    <t>v0169</t>
+  </si>
+  <si>
+    <t>userType20</t>
+  </si>
+  <si>
+    <t>0362</t>
+  </si>
+  <si>
+    <t>Arul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1960,6 +2331,55 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2043,7 +2463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2146,16 +2566,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -2233,61 +2674,39 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
+    <cellStyle name="Excel_20_Built-in_20_Hyperlink" xfId="4"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
+    <cellStyle name="Heading" xfId="5"/>
+    <cellStyle name="Heading1" xfId="6"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Result" xfId="7"/>
+    <cellStyle name="Result2" xfId="8"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2914,19 +3333,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3054,6 +3473,37 @@
       </c>
       <c r="D9" t="s">
         <v>478</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="68" t="s">
+        <v>741</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>742</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>306</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="68" t="s">
+        <v>743</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>744</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>306</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -3064,6 +3514,8 @@
     <hyperlink ref="C6" r:id="rId4"/>
     <hyperlink ref="C7" r:id="rId5"/>
     <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3077,16 +3529,16 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="7" max="7" width="22.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3164,31 +3616,31 @@
       <selection activeCell="C3" sqref="C3:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" style="45" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.33203125" style="45" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
   </cols>
@@ -3785,27 +4237,27 @@
       <selection activeCell="C3" sqref="C3:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1" collapsed="1"/>
     <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4203,17 +4655,17 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.6640625" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4371,21 +4823,21 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="22.44140625" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4598,11 +5050,11 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4640,22 +5092,22 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="15" thickBot="1">
       <c r="A1" s="50" t="s">
         <v>16</v>
       </c>
@@ -4690,7 +5142,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:11" ht="15" thickBot="1">
       <c r="A2" s="53" t="s">
         <v>538</v>
       </c>
@@ -4739,28 +5191,28 @@
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4898,39 +5350,39 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="28.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="28.5546875" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" customWidth="1"/>
-    <col min="19" max="19" width="31.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" customWidth="1"/>
+    <col min="19" max="19" width="31.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5546875" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" customWidth="1"/>
     <col min="25" max="25" width="9" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" customWidth="1"/>
     <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" customWidth="1"/>
-    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" customWidth="1"/>
+    <col min="28" max="28" width="8.44140625" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.5546875" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" customWidth="1"/>
+    <col min="32" max="32" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="48.75" customHeight="1">
@@ -5139,1165 +5591,231 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="22" t="s">
-        <v>491</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>492</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="B21" s="51" t="s">
-        <v>501</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="22" t="s">
-        <v>502</v>
-      </c>
-      <c r="B22" s="51" t="s">
-        <v>503</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>506</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="22" t="s">
-        <v>507</v>
-      </c>
-      <c r="B24" s="51" t="s">
-        <v>508</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="22" t="s">
-        <v>509</v>
-      </c>
-      <c r="B25" s="51" t="s">
-        <v>508</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="52" t="s">
-        <v>532</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="52" t="s">
-        <v>534</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="52" t="s">
-        <v>538</v>
-      </c>
-      <c r="B28" s="51" t="s">
-        <v>539</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="52" t="s">
-        <v>548</v>
-      </c>
-      <c r="B29" s="51" t="s">
-        <v>539</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="52" t="s">
-        <v>549</v>
-      </c>
-      <c r="B30" s="51" t="s">
-        <v>550</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="52" t="s">
-        <v>551</v>
-      </c>
-      <c r="B31" s="51" t="s">
-        <v>552</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="52" t="s">
-        <v>553</v>
-      </c>
-      <c r="B32" s="51" t="s">
-        <v>554</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="52" t="s">
-        <v>555</v>
-      </c>
-      <c r="B33" s="51" t="s">
-        <v>556</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="52" t="s">
-        <v>524</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="52" t="s">
-        <v>559</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="52" t="s">
-        <v>560</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="52" t="s">
-        <v>561</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="52" t="s">
-        <v>562</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="52" t="s">
-        <v>563</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="52" t="s">
-        <v>564</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="52" t="s">
-        <v>565</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="52" t="s">
-        <v>595</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="52" t="s">
-        <v>615</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="52" t="s">
-        <v>616</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="52" t="s">
-        <v>617</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="52" t="s">
-        <v>618</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="52" t="s">
-        <v>619</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="52" t="s">
-        <v>620</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="52" t="s">
-        <v>621</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="52" t="s">
-        <v>622</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="52" t="s">
-        <v>623</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="52" t="s">
-        <v>624</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="52" t="s">
-        <v>557</v>
-      </c>
-      <c r="B53" s="51" t="s">
-        <v>558</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="22" t="s">
-        <v>387</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>388</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="22" t="s">
-        <v>392</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="22" t="s">
-        <v>397</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="22" t="s">
-        <v>404</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>405</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="22" t="s">
-        <v>406</v>
-      </c>
-      <c r="B60" s="22" t="s">
-        <v>407</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="22" t="s">
-        <v>408</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>411</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>413</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="22" t="s">
-        <v>436</v>
-      </c>
-      <c r="B66" s="22" t="s">
-        <v>437</v>
-      </c>
-      <c r="C66" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="22" t="s">
-        <v>438</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="22" t="s">
-        <v>448</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>449</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>455</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="B70" s="22" t="s">
-        <v>460</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="22" t="s">
-        <v>463</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>464</v>
-      </c>
-      <c r="C71" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="C72" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>469</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="42" t="s">
-        <v>326</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="42" t="s">
-        <v>329</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>330</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="42" t="s">
-        <v>331</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="42" t="s">
-        <v>335</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="42" t="s">
-        <v>347</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="C79" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="42" t="s">
-        <v>338</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="B87" s="33"/>
-      <c r="C87" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="B88" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="B89" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="B91" s="36"/>
-      <c r="C91" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="B92" s="37" t="s">
-        <v>296</v>
-      </c>
-      <c r="C92" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C93" s="20" t="s">
-        <v>75</v>
-      </c>
+    <row r="1" spans="1:11">
+      <c r="A1" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>677</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>678</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>679</v>
+      </c>
+      <c r="I1" s="57" t="s">
+        <v>680</v>
+      </c>
+      <c r="J1" s="57" t="s">
+        <v>681</v>
+      </c>
+      <c r="K1" s="57" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="55" t="s">
+        <v>625</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>626</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="G2" s="59">
+        <v>232366</v>
+      </c>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="19" t="s">
+        <v>684</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="55" t="s">
+        <v>627</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>628</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="55" t="s">
+        <v>629</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>630</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="G4" s="59">
+        <v>595959</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="55" t="s">
+        <v>631</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>632</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="55" t="s">
+        <v>633</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>634</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="55" t="s">
+        <v>635</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>636</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="55" t="s">
+        <v>637</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>638</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>541</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="G9" s="60"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="G11" s="60"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C20:C53">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C19">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C93">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C53">
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C53">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C53">
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C31">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C31">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C52">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C37">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C37">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:C52">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:C46">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C93">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6309,40 +5827,40 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.6640625" style="4" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.88671875" style="4" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="29" max="29" width="31.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6700,21 +6218,2233 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>690</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>691</v>
+      </c>
+      <c r="H1" s="62" t="s">
+        <v>692</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>693</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>694</v>
+      </c>
+      <c r="K1" s="62" t="s">
+        <v>695</v>
+      </c>
+      <c r="L1" s="62" t="s">
+        <v>696</v>
+      </c>
+      <c r="M1" s="62" t="s">
+        <v>697</v>
+      </c>
+      <c r="N1" s="62" t="s">
+        <v>698</v>
+      </c>
+      <c r="O1" s="62" t="s">
+        <v>699</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q1" s="62" t="s">
+        <v>701</v>
+      </c>
+      <c r="R1" s="62" t="s">
+        <v>702</v>
+      </c>
+      <c r="S1" s="62" t="s">
+        <v>703</v>
+      </c>
+      <c r="T1" s="62" t="s">
+        <v>704</v>
+      </c>
+      <c r="U1" s="62" t="s">
+        <v>325</v>
+      </c>
+      <c r="V1" s="62" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="55" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="63">
+        <v>45239</v>
+      </c>
+      <c r="L2" s="20">
+        <v>55</v>
+      </c>
+      <c r="M2" s="20">
+        <v>12</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>709</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="P2" s="20">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="63">
+        <v>45239</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>711</v>
+      </c>
+      <c r="S2" s="20">
+        <v>15</v>
+      </c>
+      <c r="T2" s="20">
+        <v>22</v>
+      </c>
+      <c r="U2" s="20" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="55" t="s">
+        <v>641</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>642</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20" t="s">
+        <v>686</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="55" t="s">
+        <v>643</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>644</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="55" t="s">
+        <v>645</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>646</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="55" t="s">
+        <v>647</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>648</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="55" t="s">
+        <v>649</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>650</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>715</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="K7" s="63">
+        <v>45239</v>
+      </c>
+      <c r="L7" s="20">
+        <v>66</v>
+      </c>
+      <c r="M7" s="20">
+        <v>23</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="P7" s="20">
+        <v>99</v>
+      </c>
+      <c r="Q7" s="63">
+        <v>45239</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>719</v>
+      </c>
+      <c r="S7" s="20">
+        <v>23</v>
+      </c>
+      <c r="T7" s="20">
+        <v>44</v>
+      </c>
+      <c r="U7" s="20" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="55" t="s">
+        <v>651</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20" t="s">
+        <v>721</v>
+      </c>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1"/>
+    <hyperlink ref="V3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>724</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>725</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>726</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="24" t="s">
+        <v>653</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>654</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="24" t="s">
+        <v>655</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>656</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="24" t="s">
+        <v>657</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>658</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="G4" s="20">
+        <v>4343</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>732</v>
+      </c>
+      <c r="J4" s="20">
+        <v>55555</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="24" t="s">
+        <v>659</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>660</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="24" t="s">
+        <v>661</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>662</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="G6" s="20">
+        <v>5656</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>735</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="J6" s="20">
+        <v>77777</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="24" t="s">
+        <v>663</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>664</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="20" t="s">
+        <v>737</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="24" t="s">
+        <v>665</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>666</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>671</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="22" t="s">
+        <v>673</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>674</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="22" t="s">
+        <v>675</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>676</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>683</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="22" t="s">
+        <v>667</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="C2" s="20">
+        <v>4006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H119"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.44140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>492</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>501</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>503</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>506</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>508</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>508</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="55" t="s">
+        <v>625</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>626</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="55" t="s">
+        <v>627</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>628</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="55" t="s">
+        <v>629</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>630</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="55" t="s">
+        <v>631</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>632</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="55" t="s">
+        <v>633</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>634</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="55" t="s">
+        <v>635</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>636</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="55" t="s">
+        <v>637</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>638</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="55" t="s">
+        <v>639</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="55" t="s">
+        <v>641</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>642</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="55" t="s">
+        <v>643</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>644</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="55" t="s">
+        <v>645</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>646</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="55" t="s">
+        <v>647</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>648</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="55" t="s">
+        <v>649</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>650</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="55" t="s">
+        <v>651</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="22" t="s">
+        <v>661</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="22" t="s">
+        <v>663</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="22" t="s">
+        <v>665</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>666</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="22" t="s">
+        <v>667</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="22" t="s">
+        <v>671</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="22" t="s">
+        <v>673</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>674</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="22" t="s">
+        <v>675</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>676</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="52" t="s">
+        <v>532</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="52" t="s">
+        <v>534</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="52" t="s">
+        <v>538</v>
+      </c>
+      <c r="B54" s="51" t="s">
+        <v>539</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="52" t="s">
+        <v>548</v>
+      </c>
+      <c r="B55" s="51" t="s">
+        <v>539</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="52" t="s">
+        <v>549</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>550</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="52" t="s">
+        <v>551</v>
+      </c>
+      <c r="B57" s="51" t="s">
+        <v>552</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="52" t="s">
+        <v>553</v>
+      </c>
+      <c r="B58" s="51" t="s">
+        <v>554</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="52" t="s">
+        <v>555</v>
+      </c>
+      <c r="B59" s="51" t="s">
+        <v>556</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="52" t="s">
+        <v>524</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="52" t="s">
+        <v>559</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="52" t="s">
+        <v>560</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="52" t="s">
+        <v>561</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="52" t="s">
+        <v>562</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="52" t="s">
+        <v>563</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="52" t="s">
+        <v>564</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="52" t="s">
+        <v>565</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="52" t="s">
+        <v>595</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="52" t="s">
+        <v>615</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="52" t="s">
+        <v>616</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="52" t="s">
+        <v>617</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="52" t="s">
+        <v>618</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="52" t="s">
+        <v>619</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="52" t="s">
+        <v>621</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="52" t="s">
+        <v>622</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="52" t="s">
+        <v>623</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="52" t="s">
+        <v>624</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="52" t="s">
+        <v>557</v>
+      </c>
+      <c r="B79" s="51" t="s">
+        <v>558</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C88" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="42" t="s">
+        <v>335</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="42" t="s">
+        <v>347</v>
+      </c>
+      <c r="B105" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B110" s="18"/>
+      <c r="C110" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C111" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B113" s="33"/>
+      <c r="C113" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C114" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C115" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B117" s="36"/>
+      <c r="C117" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="B118" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="C118" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C119" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C119">
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80:C119">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C119">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C119">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C119">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C57">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C78">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C63">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C63">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C78">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C72">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:C119">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79:C119">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C119">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6847,18 +8577,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -7235,26 +8965,26 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.33203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.109375" style="4" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.44140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5546875" style="4" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="19" max="16384" width="9.109375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -7461,30 +9191,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.88671875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.33203125" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.44140625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -7693,25 +9423,25 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -7935,30 +9665,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -8179,13 +9909,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8279,11 +10009,11 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
JSE click changes commit and test data updated
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="23256" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="17" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="747">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1462,12 +1462,6 @@
     <t>0354</t>
   </si>
   <si>
-    <t>5315</t>
-  </si>
-  <si>
-    <t>0315</t>
-  </si>
-  <si>
     <t>userType07</t>
   </si>
   <si>
@@ -2276,6 +2270,15 @@
   </si>
   <si>
     <t>Arul</t>
+  </si>
+  <si>
+    <t>10:10</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>4006</t>
   </si>
 </sst>
 </file>
@@ -2596,7 +2599,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -2694,6 +2697,10 @@
     <xf numFmtId="49" fontId="9" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Excel_20_Built-in_20_Hyperlink" xfId="4"/>
@@ -3335,17 +3342,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3420,7 +3427,7 @@
         <v>340</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>475</v>
+        <v>311</v>
       </c>
       <c r="C6" s="39" t="s">
         <v>306</v>
@@ -3463,47 +3470,47 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="38" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>306</v>
       </c>
       <c r="D9" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="68" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>306</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="68" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C11" s="68" t="s">
         <v>306</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -3529,16 +3536,16 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.44140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3616,31 +3623,31 @@
       <selection activeCell="C3" sqref="C3:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.33203125" style="45" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" style="45" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
   </cols>
@@ -4237,27 +4244,27 @@
       <selection activeCell="C3" sqref="C3:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
     <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4655,17 +4662,17 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.7109375" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4819,221 +4826,222 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="69" t="s">
+        <v>477</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>478</v>
+      </c>
+      <c r="E1" s="69" t="s">
         <v>479</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="50" t="s">
+      <c r="F1" s="69" t="s">
         <v>480</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="G1" s="69" t="s">
         <v>481</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="H1" s="69" t="s">
         <v>482</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="I1" s="69" t="s">
         <v>483</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="J1" s="69" t="s">
         <v>484</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="K1" s="69" t="s">
         <v>485</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="L1" s="69" t="s">
         <v>486</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="M1" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="N1" s="69" t="s">
         <v>488</v>
       </c>
-      <c r="M1" s="50" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="70" t="s">
         <v>489</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="B2" s="70" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="51" t="s">
+      <c r="C2" s="7">
+        <v>5301</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="E2" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="C2" s="20">
+      <c r="F2" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="M2" s="7">
+        <v>-987456321</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="70" t="s">
+        <v>498</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="C3" s="7">
         <v>5301</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>494</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="H2" s="20">
-        <v>0.4236111111111111</v>
-      </c>
-      <c r="I2" s="20" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="L3" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="M3" s="7">
+        <v>-9875632</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="M2" s="20">
-        <v>-987456321</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="51" t="s">
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="70" t="s">
         <v>500</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B4" s="70" t="s">
         <v>501</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C4" s="7">
         <v>5301</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="M3" s="20">
-        <v>-9875632</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="51" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="70" t="s">
         <v>503</v>
       </c>
-      <c r="C4" s="20">
+      <c r="B5" s="70" t="s">
+        <v>504</v>
+      </c>
+      <c r="C5" s="7">
         <v>5301</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="51" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="70" t="s">
         <v>505</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B6" s="70" t="s">
         <v>506</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C6" s="7">
         <v>5301</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="51" t="s">
-        <v>507</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>508</v>
-      </c>
-      <c r="C6" s="20">
-        <v>5301</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="M6" s="20">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="M6" s="7">
         <f>M3-987456321</f>
         <v>-997331953</v>
       </c>
-      <c r="N6" s="20" t="s">
-        <v>499</v>
+      <c r="N6" s="7" t="s">
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -5050,11 +5058,11 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5062,18 +5070,18 @@
         <v>16</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="52" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C2" s="20">
         <v>5301</v>
@@ -5092,30 +5100,30 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="50" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D1" s="50" t="s">
         <v>4</v>
@@ -5124,10 +5132,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>29</v>
@@ -5142,39 +5150,39 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="53" t="s">
+        <v>536</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="D2" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>543</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>545</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -5191,28 +5199,28 @@
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5220,55 +5228,55 @@
         <v>16</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D1" s="50" t="s">
         <v>318</v>
       </c>
       <c r="E1" s="50" t="s">
+        <v>509</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>511</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>512</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>513</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>432</v>
       </c>
       <c r="I1" s="50" t="s">
+        <v>512</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>513</v>
+      </c>
+      <c r="K1" s="50" t="s">
         <v>514</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>515</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="M1" s="50" t="s">
         <v>516</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="N1" s="50" t="s">
         <v>517</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="O1" s="50" t="s">
         <v>518</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="P1" s="50" t="s">
         <v>519</v>
       </c>
-      <c r="O1" s="50" t="s">
+      <c r="Q1" s="50" t="s">
         <v>520</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="R1" s="50" t="s">
         <v>521</v>
-      </c>
-      <c r="Q1" s="50" t="s">
-        <v>522</v>
-      </c>
-      <c r="R1" s="50" t="s">
-        <v>523</v>
       </c>
       <c r="S1" s="50" t="s">
         <v>425</v>
@@ -5279,10 +5287,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C2" s="20">
         <v>5301</v>
@@ -5297,7 +5305,7 @@
         <v>13000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>453</v>
@@ -5313,13 +5321,13 @@
         <v>297</v>
       </c>
       <c r="M2" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>527</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>528</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>529</v>
       </c>
       <c r="P2" s="20" t="s">
         <v>453</v>
@@ -5331,10 +5339,10 @@
         <v>100</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -5350,39 +5358,39 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="10" width="29.44140625" customWidth="1"/>
-    <col min="11" max="11" width="28.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" customWidth="1"/>
-    <col min="14" max="14" width="28.5546875" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" customWidth="1"/>
-    <col min="16" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" customWidth="1"/>
-    <col min="19" max="19" width="31.6640625" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5546875" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" customWidth="1"/>
-    <col min="25" max="25" width="9" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" customWidth="1"/>
-    <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="8.44140625" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5546875" customWidth="1"/>
-    <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="9" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="9" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.42578125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="48.75" customHeight="1">
@@ -5390,108 +5398,108 @@
         <v>316</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C1" s="54" t="s">
+        <v>564</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="F1" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="G1" s="54" t="s">
         <v>568</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="H1" s="54" t="s">
         <v>569</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="I1" s="54" t="s">
         <v>570</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="J1" s="54" t="s">
         <v>571</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="K1" s="54" t="s">
         <v>572</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="L1" s="54" t="s">
         <v>573</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="M1" s="54" t="s">
         <v>574</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="N1" s="54" t="s">
         <v>575</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="O1" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="P1" s="54" t="s">
         <v>577</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="Q1" s="54" t="s">
         <v>578</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="R1" s="54" t="s">
         <v>579</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="S1" s="54" t="s">
         <v>580</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="T1" s="54" t="s">
         <v>581</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="U1" s="54" t="s">
         <v>582</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="V1" s="54" t="s">
         <v>583</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="W1" s="54" t="s">
         <v>584</v>
       </c>
-      <c r="V1" s="54" t="s">
+      <c r="X1" s="54" t="s">
         <v>585</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="Y1" s="54" t="s">
         <v>586</v>
-      </c>
-      <c r="X1" s="54" t="s">
-        <v>587</v>
-      </c>
-      <c r="Y1" s="54" t="s">
-        <v>588</v>
       </c>
       <c r="Z1" s="54" t="s">
         <v>361</v>
       </c>
       <c r="AA1" s="54" t="s">
+        <v>587</v>
+      </c>
+      <c r="AB1" s="54" t="s">
+        <v>588</v>
+      </c>
+      <c r="AC1" s="54" t="s">
         <v>589</v>
       </c>
-      <c r="AB1" s="54" t="s">
+      <c r="AD1" s="54" t="s">
         <v>590</v>
       </c>
-      <c r="AC1" s="54" t="s">
+      <c r="AE1" s="54" t="s">
         <v>591</v>
       </c>
-      <c r="AD1" s="54" t="s">
+      <c r="AF1" s="54" t="s">
         <v>592</v>
-      </c>
-      <c r="AE1" s="54" t="s">
-        <v>593</v>
-      </c>
-      <c r="AF1" s="54" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>595</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>597</v>
       </c>
       <c r="D2" s="20">
         <v>9574315615</v>
@@ -5500,25 +5508,25 @@
         <v>32</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>598</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>599</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>600</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>600</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>601</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>602</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>603</v>
       </c>
       <c r="M2" s="20">
         <v>1234</v>
@@ -5527,16 +5535,16 @@
         <v>32</v>
       </c>
       <c r="O2" s="20" t="s">
+        <v>602</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q2" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="P2" s="20" t="s">
-        <v>605</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>606</v>
-      </c>
       <c r="R2" s="20" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="S2" s="20">
         <v>10000</v>
@@ -5548,37 +5556,37 @@
         <v>10000</v>
       </c>
       <c r="V2" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="X2" s="20" t="s">
         <v>607</v>
-      </c>
-      <c r="W2" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>609</v>
       </c>
       <c r="Y2" s="20" t="s">
         <v>160</v>
       </c>
       <c r="Z2" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="AC2" s="20" t="s">
         <v>610</v>
       </c>
-      <c r="AA2" s="20" t="s">
-        <v>610</v>
-      </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>611</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>612</v>
-      </c>
-      <c r="AD2" s="20" t="s">
-        <v>613</v>
       </c>
       <c r="AE2" s="20">
         <v>10000</v>
       </c>
       <c r="AF2" s="20" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -5597,18 +5605,18 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5628,38 +5636,38 @@
         <v>130</v>
       </c>
       <c r="F1" s="57" t="s">
+        <v>675</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>676</v>
+      </c>
+      <c r="H1" s="57" t="s">
         <v>677</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>678</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>680</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>681</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="55" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="G2" s="59">
         <v>232366</v>
@@ -5667,27 +5675,27 @@
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="19" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="55" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D3" s="58"/>
       <c r="E3" s="58"/>
       <c r="F3" s="58"/>
       <c r="G3" s="19" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H3" s="58"/>
       <c r="I3" s="58"/>
@@ -5696,18 +5704,18 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="55" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
       <c r="F4" s="19" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G4" s="59">
         <v>595959</v>
@@ -5715,27 +5723,27 @@
       <c r="H4" s="58"/>
       <c r="I4" s="58"/>
       <c r="J4" s="19" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="55" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
       <c r="G5" s="19" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
@@ -5744,13 +5752,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="55" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D6" s="58"/>
       <c r="E6" s="58"/>
@@ -5763,13 +5771,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="55" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D7" s="58"/>
       <c r="E7" s="58"/>
@@ -5782,19 +5790,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="55" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="58"/>
@@ -5827,40 +5835,40 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.88671875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6120,7 +6128,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>474</v>
+        <v>745</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -6224,29 +6232,29 @@
       <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -6267,77 +6275,77 @@
         <v>130</v>
       </c>
       <c r="F1" s="62" t="s">
+        <v>688</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>689</v>
+      </c>
+      <c r="H1" s="62" t="s">
         <v>690</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="I1" s="62" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="J1" s="62" t="s">
         <v>692</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>693</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="L1" s="62" t="s">
         <v>694</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="M1" s="62" t="s">
         <v>695</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="N1" s="62" t="s">
         <v>696</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="O1" s="62" t="s">
         <v>697</v>
       </c>
-      <c r="N1" s="62" t="s">
+      <c r="P1" s="62" t="s">
         <v>698</v>
       </c>
-      <c r="O1" s="62" t="s">
+      <c r="Q1" s="62" t="s">
         <v>699</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="R1" s="62" t="s">
         <v>700</v>
       </c>
-      <c r="Q1" s="62" t="s">
+      <c r="S1" s="62" t="s">
         <v>701</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="T1" s="62" t="s">
         <v>702</v>
-      </c>
-      <c r="S1" s="62" t="s">
-        <v>703</v>
-      </c>
-      <c r="T1" s="62" t="s">
-        <v>704</v>
       </c>
       <c r="U1" s="62" t="s">
         <v>325</v>
       </c>
       <c r="V1" s="62" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="55" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>705</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>706</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>708</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>195</v>
@@ -6355,10 +6363,10 @@
         <v>12</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="P2" s="20">
         <v>44</v>
@@ -6367,7 +6375,7 @@
         <v>45239</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="S2" s="20">
         <v>15</v>
@@ -6376,18 +6384,18 @@
         <v>22</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="55" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -6401,7 +6409,7 @@
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>
       <c r="O3" s="20" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="20"/>
@@ -6410,18 +6418,18 @@
       <c r="T3" s="20"/>
       <c r="U3" s="20"/>
       <c r="V3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="55" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -6444,13 +6452,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="55" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -6473,19 +6481,19 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="55" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -6506,27 +6514,27 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="55" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G7" s="20" t="s">
+        <v>712</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>714</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>715</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>716</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>297</v>
@@ -6541,10 +6549,10 @@
         <v>23</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="P7" s="20">
         <v>99</v>
@@ -6553,7 +6561,7 @@
         <v>45239</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="S7" s="20">
         <v>23</v>
@@ -6562,18 +6570,18 @@
         <v>44</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="55" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -6587,7 +6595,7 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
@@ -6613,19 +6621,19 @@
       <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6645,33 +6653,33 @@
         <v>130</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>720</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>723</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>724</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>725</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>726</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="24" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -6684,19 +6692,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="24" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -6707,49 +6715,49 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="24" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="20" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G4" s="20">
         <v>4343</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J4" s="20">
         <v>55555</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="24" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="20" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -6759,27 +6767,27 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="24" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="20" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G6" s="20">
         <v>5656</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="J6" s="20">
         <v>77777</v>
@@ -6790,18 +6798,18 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="24" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="20" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
@@ -6811,13 +6819,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="24" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -6838,17 +6846,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6870,56 +6878,56 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>683</v>
+        <v>746</v>
       </c>
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>683</v>
+        <v>746</v>
       </c>
       <c r="D3" s="58"/>
       <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>683</v>
+        <v>746</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>683</v>
+        <v>746</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="58"/>
@@ -6934,13 +6942,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C8"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6948,7 +6956,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>318</v>
@@ -6956,10 +6964,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="22" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C2" s="20">
         <v>4006</v>
@@ -6978,16 +6986,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7214,10 +7222,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="22" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>24</v>
@@ -7225,10 +7233,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="22" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>24</v>
@@ -7236,10 +7244,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="22" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>24</v>
@@ -7247,10 +7255,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="22" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>24</v>
@@ -7258,10 +7266,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="22" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>24</v>
@@ -7269,10 +7277,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>24</v>
@@ -7280,10 +7288,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="55" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B26" s="55" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>24</v>
@@ -7291,10 +7299,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="55" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>24</v>
@@ -7302,10 +7310,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="55" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B28" s="55" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>24</v>
@@ -7313,10 +7321,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="55" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B29" s="55" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>24</v>
@@ -7324,10 +7332,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="55" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>24</v>
@@ -7335,10 +7343,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="55" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>24</v>
@@ -7346,10 +7354,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="55" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>24</v>
@@ -7357,10 +7365,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="55" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>24</v>
@@ -7368,10 +7376,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="55" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>24</v>
@@ -7379,10 +7387,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="55" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B35" s="55" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>24</v>
@@ -7390,10 +7398,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="55" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B36" s="55" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>24</v>
@@ -7401,10 +7409,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="55" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>24</v>
@@ -7412,10 +7420,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="55" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B38" s="55" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>24</v>
@@ -7423,10 +7431,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="55" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B39" s="55" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>24</v>
@@ -7434,10 +7442,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="22" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>24</v>
@@ -7445,10 +7453,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="22" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>24</v>
@@ -7456,10 +7464,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="22" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>24</v>
@@ -7467,10 +7475,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="22" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>24</v>
@@ -7478,10 +7486,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="22" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>24</v>
@@ -7489,10 +7497,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="22" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>24</v>
@@ -7500,10 +7508,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="22" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>24</v>
@@ -7511,10 +7519,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="22" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>24</v>
@@ -7522,10 +7530,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>24</v>
@@ -7533,10 +7541,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="22" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>24</v>
@@ -7544,10 +7552,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>24</v>
@@ -7555,10 +7563,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>24</v>
@@ -7566,10 +7574,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="52" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>24</v>
@@ -7577,10 +7585,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="52" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>24</v>
@@ -7588,10 +7596,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="52" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B54" s="51" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>24</v>
@@ -7599,10 +7607,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="52" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B55" s="51" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>24</v>
@@ -7610,10 +7618,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="52" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>24</v>
@@ -7621,10 +7629,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="52" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>24</v>
@@ -7632,10 +7640,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="52" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B58" s="51" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>24</v>
@@ -7643,10 +7651,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="52" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B59" s="51" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>24</v>
@@ -7654,10 +7662,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="52" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>24</v>
@@ -7665,10 +7673,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="52" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>24</v>
@@ -7676,10 +7684,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="52" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>24</v>
@@ -7687,10 +7695,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="52" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>24</v>
@@ -7698,10 +7706,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="52" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>24</v>
@@ -7709,10 +7717,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="52" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C65" s="20" t="s">
         <v>24</v>
@@ -7720,10 +7728,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="52" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>24</v>
@@ -7731,10 +7739,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="52" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C67" s="20" t="s">
         <v>24</v>
@@ -7742,10 +7750,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="52" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>24</v>
@@ -7753,10 +7761,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="52" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C69" s="20" t="s">
         <v>24</v>
@@ -7764,10 +7772,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="52" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C70" s="20" t="s">
         <v>24</v>
@@ -7775,10 +7783,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="52" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>24</v>
@@ -7786,10 +7794,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="52" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>24</v>
@@ -7797,10 +7805,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="52" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>24</v>
@@ -7808,10 +7816,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="52" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>24</v>
@@ -7819,10 +7827,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="52" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C75" s="20" t="s">
         <v>24</v>
@@ -7830,10 +7838,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="52" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C76" s="20" t="s">
         <v>24</v>
@@ -7841,10 +7849,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="52" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C77" s="20" t="s">
         <v>24</v>
@@ -7852,10 +7860,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="52" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>24</v>
@@ -7863,10 +7871,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="52" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>24</v>
@@ -8436,15 +8444,15 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8577,18 +8585,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -8965,26 +8973,26 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.6640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -9191,30 +9199,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.88671875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.109375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.44140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -9423,25 +9431,25 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -9665,30 +9673,30 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -9909,13 +9917,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10009,11 +10017,11 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Auto loan - Underwriter,Financial commitments, Appication details testcases updated
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="768">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -3423,11 +3423,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.49609375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
+    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3613,14 +3613,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3700,31 +3700,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" style="44" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="44" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -4321,25 +4321,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4739,15 +4739,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="44" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="44" width="25.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4907,20 +4907,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5134,9 +5134,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5176,17 +5176,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
@@ -5275,26 +5275,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5434,37 +5434,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="28.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" customWidth="1"/>
-    <col min="19" max="19" width="31.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" customWidth="1"/>
-    <col min="25" max="25" width="9" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" customWidth="1"/>
-    <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" customWidth="1"/>
-    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" customWidth="1"/>
-    <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="48.75" customHeight="1">
@@ -5681,16 +5681,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5911,38 +5911,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
+    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6308,28 +6308,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -6697,17 +6697,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6926,11 +6926,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7021,8 +7021,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7062,11 +7062,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7135,11 +7135,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7208,11 +7208,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7281,14 +7281,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8805,13 +8805,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8946,16 +8946,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
+    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -9334,24 +9334,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -9560,28 +9560,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -9792,23 +9792,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10034,28 +10034,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -10278,11 +10278,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10378,9 +10378,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Income details contact and identification updated code commit User ID: Gowtham
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="25" activeTab="27"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -39,12 +39,12 @@
     <sheet name="AutoLoanExecution" sheetId="2" r:id="rId30"/>
     <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId31"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="857">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1684,9 +1684,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>8745632147856</t>
-  </si>
-  <si>
     <t>abcdef</t>
   </si>
   <si>
@@ -2612,6 +2609,12 @@
   </si>
   <si>
     <t>9652147856</t>
+  </si>
+  <si>
+    <t>10:05</t>
+  </si>
+  <si>
+    <t>4566</t>
   </si>
 </sst>
 </file>
@@ -3606,40 +3609,40 @@
         <v>478</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="67" t="s">
+        <v>740</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>741</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>742</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>306</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="67" t="s">
+        <v>742</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>743</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>744</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>306</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>477</v>
@@ -3648,21 +3651,21 @@
         <v>306</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>306</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -4980,8 +4983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5068,8 +5071,8 @@
       <c r="G2" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="H2" s="20">
-        <v>0.4236111111111111</v>
+      <c r="H2" s="7" t="s">
+        <v>855</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>495</v>
@@ -5332,10 +5335,10 @@
         <v>31</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>546</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -5348,8 +5351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5466,7 +5469,9 @@
       <c r="I2" s="20">
         <v>85000</v>
       </c>
-      <c r="J2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>250</v>
+      </c>
       <c r="K2" s="20">
         <v>100</v>
       </c>
@@ -5554,105 +5559,105 @@
         <v>479</v>
       </c>
       <c r="C1" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>566</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="E1" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="F1" s="53" t="s">
         <v>568</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="G1" s="53" t="s">
         <v>569</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="H1" s="53" t="s">
         <v>570</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="I1" s="53" t="s">
         <v>571</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="J1" s="53" t="s">
         <v>572</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="K1" s="53" t="s">
         <v>573</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="53" t="s">
         <v>574</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="M1" s="53" t="s">
         <v>575</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="N1" s="53" t="s">
         <v>576</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="O1" s="53" t="s">
         <v>577</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="P1" s="53" t="s">
         <v>578</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="Q1" s="53" t="s">
         <v>579</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="R1" s="53" t="s">
         <v>580</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="S1" s="53" t="s">
         <v>581</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="T1" s="53" t="s">
         <v>582</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="U1" s="53" t="s">
         <v>583</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="V1" s="53" t="s">
         <v>584</v>
       </c>
-      <c r="V1" s="53" t="s">
+      <c r="W1" s="53" t="s">
         <v>585</v>
       </c>
-      <c r="W1" s="53" t="s">
+      <c r="X1" s="53" t="s">
         <v>586</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="Y1" s="53" t="s">
         <v>587</v>
-      </c>
-      <c r="Y1" s="53" t="s">
-        <v>588</v>
       </c>
       <c r="Z1" s="53" t="s">
         <v>361</v>
       </c>
       <c r="AA1" s="53" t="s">
+        <v>588</v>
+      </c>
+      <c r="AB1" s="53" t="s">
         <v>589</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>590</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="53" t="s">
         <v>591</v>
       </c>
-      <c r="AD1" s="53" t="s">
+      <c r="AE1" s="53" t="s">
         <v>592</v>
       </c>
-      <c r="AE1" s="53" t="s">
+      <c r="AF1" s="53" t="s">
         <v>593</v>
-      </c>
-      <c r="AF1" s="53" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>596</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>597</v>
       </c>
       <c r="D2" s="20">
         <v>9574315615</v>
@@ -5661,25 +5666,25 @@
         <v>32</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>598</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>599</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>600</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>601</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="7" t="s">
         <v>602</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>603</v>
       </c>
       <c r="M2" s="20">
         <v>1234</v>
@@ -5688,16 +5693,16 @@
         <v>32</v>
       </c>
       <c r="O2" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="P2" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="20" t="s">
         <v>605</v>
       </c>
-      <c r="Q2" s="20" t="s">
-        <v>606</v>
-      </c>
       <c r="R2" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S2" s="20">
         <v>10000</v>
@@ -5709,37 +5714,37 @@
         <v>10000</v>
       </c>
       <c r="V2" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="W2" s="20" t="s">
         <v>607</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>608</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>609</v>
       </c>
       <c r="Y2" s="20" t="s">
         <v>160</v>
       </c>
       <c r="Z2" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="AB2" s="20" t="s">
         <v>610</v>
       </c>
-      <c r="AA2" s="20" t="s">
-        <v>610</v>
-      </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AC2" s="20" t="s">
         <v>611</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>612</v>
-      </c>
-      <c r="AD2" s="20" t="s">
-        <v>613</v>
       </c>
       <c r="AE2" s="20">
         <v>10000</v>
       </c>
       <c r="AF2" s="20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -5789,33 +5794,33 @@
         <v>130</v>
       </c>
       <c r="F1" s="56" t="s">
+        <v>676</v>
+      </c>
+      <c r="G1" s="56" t="s">
         <v>677</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>678</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="I1" s="56" t="s">
         <v>679</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="J1" s="56" t="s">
         <v>680</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="K1" s="56" t="s">
         <v>681</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="54" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>625</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>626</v>
-      </c>
       <c r="C2" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -5828,27 +5833,27 @@
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
       <c r="J2" s="19" t="s">
+        <v>683</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>684</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="54" t="s">
+        <v>626</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>627</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>628</v>
-      </c>
       <c r="C3" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
       <c r="F3" s="57"/>
       <c r="G3" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -5857,18 +5862,18 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>629</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>630</v>
-      </c>
       <c r="C4" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="57"/>
       <c r="F4" s="19" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G4" s="58">
         <v>595959</v>
@@ -5876,7 +5881,7 @@
       <c r="H4" s="57"/>
       <c r="I4" s="57"/>
       <c r="J4" s="19" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K4" s="19" t="s">
         <v>544</v>
@@ -5884,19 +5889,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="54" t="s">
+        <v>630</v>
+      </c>
+      <c r="B5" s="54" t="s">
         <v>631</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>632</v>
-      </c>
       <c r="C5" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>
       <c r="F5" s="57"/>
       <c r="G5" s="19" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57"/>
@@ -5905,13 +5910,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" s="54" t="s">
         <v>633</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>634</v>
-      </c>
       <c r="C6" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
@@ -5924,13 +5929,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="54" t="s">
+        <v>634</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>635</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>636</v>
-      </c>
       <c r="C7" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
@@ -5943,19 +5948,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="54" t="s">
+        <v>636</v>
+      </c>
+      <c r="B8" s="54" t="s">
         <v>637</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>638</v>
-      </c>
       <c r="C8" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>541</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F8" s="57"/>
       <c r="G8" s="57"/>
@@ -6428,77 +6433,77 @@
         <v>130</v>
       </c>
       <c r="F1" s="61" t="s">
+        <v>689</v>
+      </c>
+      <c r="G1" s="61" t="s">
         <v>690</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="H1" s="61" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="I1" s="61" t="s">
         <v>692</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="J1" s="61" t="s">
         <v>693</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="K1" s="61" t="s">
         <v>694</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="61" t="s">
         <v>695</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="M1" s="61" t="s">
         <v>696</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="N1" s="61" t="s">
         <v>697</v>
       </c>
-      <c r="N1" s="61" t="s">
+      <c r="O1" s="61" t="s">
         <v>698</v>
       </c>
-      <c r="O1" s="61" t="s">
+      <c r="P1" s="61" t="s">
         <v>699</v>
       </c>
-      <c r="P1" s="61" t="s">
+      <c r="Q1" s="61" t="s">
         <v>700</v>
       </c>
-      <c r="Q1" s="61" t="s">
+      <c r="R1" s="61" t="s">
         <v>701</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="S1" s="61" t="s">
         <v>702</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="T1" s="61" t="s">
         <v>703</v>
-      </c>
-      <c r="T1" s="61" t="s">
-        <v>704</v>
       </c>
       <c r="U1" s="61" t="s">
         <v>325</v>
       </c>
       <c r="V1" s="61" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="54" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>639</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>640</v>
-      </c>
       <c r="C2" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20" t="s">
+        <v>705</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>706</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>707</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>708</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>195</v>
@@ -6516,10 +6521,10 @@
         <v>12</v>
       </c>
       <c r="N2" s="20" t="s">
+        <v>708</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>709</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>710</v>
       </c>
       <c r="P2" s="20">
         <v>44</v>
@@ -6528,7 +6533,7 @@
         <v>45239</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="S2" s="20">
         <v>15</v>
@@ -6537,18 +6542,18 @@
         <v>22</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="54" t="s">
+        <v>640</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>641</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>642</v>
-      </c>
       <c r="C3" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -6562,7 +6567,7 @@
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>
       <c r="O3" s="20" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="20"/>
@@ -6571,18 +6576,18 @@
       <c r="T3" s="20"/>
       <c r="U3" s="20"/>
       <c r="V3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="54" t="s">
+        <v>642</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>643</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>644</v>
-      </c>
       <c r="C4" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -6605,13 +6610,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="B5" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>646</v>
-      </c>
       <c r="C5" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -6634,19 +6639,19 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B6" s="54" t="s">
         <v>647</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>648</v>
-      </c>
       <c r="C6" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -6667,27 +6672,27 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="54" t="s">
+        <v>648</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>649</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>650</v>
-      </c>
       <c r="C7" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G7" s="20" t="s">
+        <v>713</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>714</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="20" t="s">
         <v>715</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>716</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>297</v>
@@ -6702,10 +6707,10 @@
         <v>23</v>
       </c>
       <c r="N7" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="O7" s="20" t="s">
         <v>717</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>718</v>
       </c>
       <c r="P7" s="20">
         <v>99</v>
@@ -6714,7 +6719,7 @@
         <v>45239</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="S7" s="20">
         <v>23</v>
@@ -6723,18 +6728,18 @@
         <v>44</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="54" t="s">
+        <v>650</v>
+      </c>
+      <c r="B8" s="54" t="s">
         <v>651</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>652</v>
-      </c>
       <c r="C8" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -6748,7 +6753,7 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
@@ -6806,33 +6811,33 @@
         <v>130</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>723</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>724</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>725</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>726</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="24" t="s">
+        <v>652</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>653</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>654</v>
-      </c>
       <c r="C2" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -6845,19 +6850,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="24" t="s">
+        <v>654</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>655</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>656</v>
-      </c>
       <c r="C3" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>728</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>729</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -6868,49 +6873,49 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="24" t="s">
+        <v>656</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>657</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>658</v>
-      </c>
       <c r="C4" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G4" s="20">
         <v>4343</v>
       </c>
       <c r="H4" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>731</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>732</v>
       </c>
       <c r="J4" s="20">
         <v>55555</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="24" t="s">
+        <v>658</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>659</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>660</v>
-      </c>
       <c r="C5" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -6920,27 +6925,27 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="24" t="s">
+        <v>660</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>661</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>662</v>
-      </c>
       <c r="C6" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="20" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G6" s="20">
         <v>5656</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>735</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>736</v>
       </c>
       <c r="J6" s="20">
         <v>77777</v>
@@ -6951,18 +6956,18 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="24" t="s">
+        <v>662</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>663</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>664</v>
-      </c>
       <c r="C7" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="20" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
@@ -6972,13 +6977,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="24" t="s">
+        <v>664</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>665</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>666</v>
-      </c>
       <c r="C8" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -7031,56 +7036,56 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>669</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>670</v>
-      </c>
       <c r="C2" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>671</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>672</v>
-      </c>
       <c r="C3" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>673</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>674</v>
-      </c>
       <c r="C4" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D4" s="57" t="s">
+        <v>737</v>
+      </c>
+      <c r="E4" s="57" t="s">
         <v>738</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
+        <v>674</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>675</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>676</v>
-      </c>
       <c r="C5" s="43" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>
@@ -7109,7 +7114,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>318</v>
@@ -7117,10 +7122,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="22" t="s">
+        <v>666</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>667</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>668</v>
       </c>
       <c r="C2" s="20">
         <v>4006</v>
@@ -7156,10 +7161,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>745</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>746</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>747</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>38</v>
@@ -7167,13 +7172,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
+        <v>747</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>748</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>749</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>750</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>93</v>
@@ -7184,13 +7189,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
+        <v>750</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>751</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>752</v>
-      </c>
       <c r="C3" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>93</v>
@@ -7232,44 +7237,44 @@
         <v>3</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>752</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>753</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>755</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="20" t="s">
+        <v>749</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>756</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>750</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>757</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
+        <v>758</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>759</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>760</v>
-      </c>
       <c r="C3" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>757</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -7302,21 +7307,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>760</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>761</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>762</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>764</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>765</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>109</v>
@@ -7330,10 +7335,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
+        <v>765</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>766</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>767</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>109</v>
@@ -7373,18 +7378,18 @@
         <v>317</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="69" t="s">
+        <v>772</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>773</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="C2" s="70" t="s">
         <v>774</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -7396,7 +7401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7435,114 +7440,114 @@
         <v>317</v>
       </c>
       <c r="C1" s="71" t="s">
+        <v>775</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>844</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>845</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>846</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>847</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>848</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>849</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>850</v>
+      </c>
+      <c r="N1" s="71" t="s">
         <v>776</v>
       </c>
-      <c r="D1" s="71" t="s">
-        <v>566</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>845</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>846</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>847</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>848</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>849</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>850</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>851</v>
-      </c>
-      <c r="N1" s="71" t="s">
+      <c r="O1" s="18" t="s">
         <v>777</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>778</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>779</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>780</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>781</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="T1" s="18" t="s">
         <v>782</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="U1" s="18" t="s">
         <v>783</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="V1" s="18" t="s">
         <v>784</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="W1" s="18" t="s">
         <v>785</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>786</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>787</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>788</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>789</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>790</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>791</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
         <v>792</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AE1" s="18" t="s">
         <v>793</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AF1" s="18" t="s">
         <v>794</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AG1" s="18" t="s">
         <v>795</v>
-      </c>
-      <c r="AG1" s="18" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="67" t="s">
+        <v>796</v>
+      </c>
+      <c r="B2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>854</v>
+      </c>
+      <c r="D2" s="67" t="s">
         <v>797</v>
       </c>
-      <c r="B2" t="s">
-        <v>816</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>855</v>
-      </c>
-      <c r="D2" s="67" t="s">
-        <v>798</v>
-      </c>
       <c r="E2" s="67" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F2" s="67">
         <v>751</v>
@@ -7551,10 +7556,10 @@
         <v>5555</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I2" s="67" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J2" s="67">
         <v>785</v>
@@ -7563,13 +7568,13 @@
         <v>9874561230</v>
       </c>
       <c r="L2" s="37" t="s">
+        <v>852</v>
+      </c>
+      <c r="M2" s="77" t="s">
         <v>853</v>
       </c>
-      <c r="M2" s="77" t="s">
-        <v>854</v>
-      </c>
       <c r="N2" s="67" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="O2" s="67" t="s">
         <v>94</v>
@@ -7602,7 +7607,7 @@
         <v>83</v>
       </c>
       <c r="Y2" s="67" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="Z2" s="67" t="s">
         <v>79</v>
@@ -7611,10 +7616,10 @@
         <v>297</v>
       </c>
       <c r="AB2" s="67" t="s">
+        <v>800</v>
+      </c>
+      <c r="AC2" s="67" t="s">
         <v>801</v>
-      </c>
-      <c r="AC2" s="67" t="s">
-        <v>802</v>
       </c>
       <c r="AD2" s="67" t="s">
         <v>297</v>
@@ -7626,7 +7631,7 @@
         <v>999</v>
       </c>
       <c r="AG2" s="67" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -7667,48 +7672,48 @@
         <v>317</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>803</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>804</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="40" t="s">
         <v>805</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>806</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>807</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>808</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>809</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="37" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>826</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>811</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>827</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
+        <v>757</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>812</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>758</v>
-      </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>813</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>814</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>815</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>250</v>
@@ -8114,8 +8119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8420,10 +8425,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="54" t="s">
+        <v>624</v>
+      </c>
+      <c r="B26" s="54" t="s">
         <v>625</v>
-      </c>
-      <c r="B26" s="54" t="s">
-        <v>626</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>24</v>
@@ -8431,10 +8436,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="54" t="s">
+        <v>626</v>
+      </c>
+      <c r="B27" s="54" t="s">
         <v>627</v>
-      </c>
-      <c r="B27" s="54" t="s">
-        <v>628</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>24</v>
@@ -8442,10 +8447,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="B28" s="54" t="s">
         <v>629</v>
-      </c>
-      <c r="B28" s="54" t="s">
-        <v>630</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>24</v>
@@ -8453,10 +8458,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="54" t="s">
+        <v>630</v>
+      </c>
+      <c r="B29" s="54" t="s">
         <v>631</v>
-      </c>
-      <c r="B29" s="54" t="s">
-        <v>632</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>24</v>
@@ -8464,10 +8469,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="B30" s="54" t="s">
         <v>633</v>
-      </c>
-      <c r="B30" s="54" t="s">
-        <v>634</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>24</v>
@@ -8475,10 +8480,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="54" t="s">
+        <v>634</v>
+      </c>
+      <c r="B31" s="54" t="s">
         <v>635</v>
-      </c>
-      <c r="B31" s="54" t="s">
-        <v>636</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>24</v>
@@ -8486,10 +8491,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="54" t="s">
+        <v>636</v>
+      </c>
+      <c r="B32" s="54" t="s">
         <v>637</v>
-      </c>
-      <c r="B32" s="54" t="s">
-        <v>638</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>24</v>
@@ -8497,10 +8502,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="54" t="s">
+        <v>638</v>
+      </c>
+      <c r="B33" s="54" t="s">
         <v>639</v>
-      </c>
-      <c r="B33" s="54" t="s">
-        <v>640</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>24</v>
@@ -8508,10 +8513,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="54" t="s">
+        <v>640</v>
+      </c>
+      <c r="B34" s="54" t="s">
         <v>641</v>
-      </c>
-      <c r="B34" s="54" t="s">
-        <v>642</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>24</v>
@@ -8519,10 +8524,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="54" t="s">
+        <v>642</v>
+      </c>
+      <c r="B35" s="54" t="s">
         <v>643</v>
-      </c>
-      <c r="B35" s="54" t="s">
-        <v>644</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>24</v>
@@ -8530,10 +8535,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="B36" s="54" t="s">
         <v>645</v>
-      </c>
-      <c r="B36" s="54" t="s">
-        <v>646</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>24</v>
@@ -8541,10 +8546,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B37" s="54" t="s">
         <v>647</v>
-      </c>
-      <c r="B37" s="54" t="s">
-        <v>648</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>24</v>
@@ -8552,10 +8557,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="54" t="s">
+        <v>648</v>
+      </c>
+      <c r="B38" s="54" t="s">
         <v>649</v>
-      </c>
-      <c r="B38" s="54" t="s">
-        <v>650</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>24</v>
@@ -8563,10 +8568,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="54" t="s">
+        <v>650</v>
+      </c>
+      <c r="B39" s="54" t="s">
         <v>651</v>
-      </c>
-      <c r="B39" s="54" t="s">
-        <v>652</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>24</v>
@@ -8574,10 +8579,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="B40" s="22" t="s">
         <v>653</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>654</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>24</v>
@@ -8585,10 +8590,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>655</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>656</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>24</v>
@@ -8596,10 +8601,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>657</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>658</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>24</v>
@@ -8607,10 +8612,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="B43" s="22" t="s">
         <v>659</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>660</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>24</v>
@@ -8618,10 +8623,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="B44" s="22" t="s">
         <v>661</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>662</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>24</v>
@@ -8629,10 +8634,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>663</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>664</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>24</v>
@@ -8640,10 +8645,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>665</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>666</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>24</v>
@@ -8651,10 +8656,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="22" t="s">
+        <v>666</v>
+      </c>
+      <c r="B47" s="22" t="s">
         <v>667</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>668</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>24</v>
@@ -8662,10 +8667,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="B48" s="22" t="s">
         <v>669</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>670</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>24</v>
@@ -8673,10 +8678,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="B49" s="22" t="s">
         <v>671</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>672</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>24</v>
@@ -8684,10 +8689,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>673</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>674</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>24</v>
@@ -8695,10 +8700,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="22" t="s">
+        <v>674</v>
+      </c>
+      <c r="B51" s="22" t="s">
         <v>675</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>676</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>24</v>
@@ -8739,7 +8744,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="51" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B55" s="50" t="s">
         <v>539</v>
@@ -8750,10 +8755,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="51" t="s">
+        <v>548</v>
+      </c>
+      <c r="B56" s="50" t="s">
         <v>549</v>
-      </c>
-      <c r="B56" s="50" t="s">
-        <v>550</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>24</v>
@@ -8761,10 +8766,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="51" t="s">
+        <v>550</v>
+      </c>
+      <c r="B57" s="50" t="s">
         <v>551</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>552</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>24</v>
@@ -8772,10 +8777,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="51" t="s">
+        <v>552</v>
+      </c>
+      <c r="B58" s="50" t="s">
         <v>553</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>554</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>24</v>
@@ -8783,10 +8788,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="51" t="s">
+        <v>554</v>
+      </c>
+      <c r="B59" s="50" t="s">
         <v>555</v>
-      </c>
-      <c r="B59" s="50" t="s">
-        <v>556</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>24</v>
@@ -8805,7 +8810,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="51" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>525</v>
@@ -8816,7 +8821,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="51" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>525</v>
@@ -8827,7 +8832,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="51" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>525</v>
@@ -8838,7 +8843,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="51" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B64" s="22" t="s">
         <v>525</v>
@@ -8849,7 +8854,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="51" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>525</v>
@@ -8860,7 +8865,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="51" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>525</v>
@@ -8871,7 +8876,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="51" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B67" s="22" t="s">
         <v>525</v>
@@ -8882,10 +8887,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="51" t="s">
+        <v>594</v>
+      </c>
+      <c r="B68" s="22" t="s">
         <v>595</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>596</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>24</v>
@@ -8893,10 +8898,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="51" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C69" s="20" t="s">
         <v>24</v>
@@ -8904,10 +8909,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="51" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C70" s="20" t="s">
         <v>24</v>
@@ -8915,10 +8920,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="51" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>24</v>
@@ -8926,10 +8931,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="51" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>24</v>
@@ -8937,10 +8942,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>24</v>
@@ -8948,10 +8953,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="51" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>24</v>
@@ -8959,10 +8964,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="51" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C75" s="20" t="s">
         <v>24</v>
@@ -8970,10 +8975,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="51" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C76" s="20" t="s">
         <v>24</v>
@@ -8981,10 +8986,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="51" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C77" s="20" t="s">
         <v>24</v>
@@ -8992,10 +8997,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="51" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>24</v>
@@ -9003,10 +9008,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="51" t="s">
+        <v>556</v>
+      </c>
+      <c r="B79" s="50" t="s">
         <v>557</v>
-      </c>
-      <c r="B79" s="50" t="s">
-        <v>558</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>24</v>
@@ -9245,10 +9250,10 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="72" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B101" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C101" s="20" t="s">
         <v>24</v>
@@ -9256,10 +9261,10 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="73" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B102" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C102" s="20" t="s">
         <v>24</v>
@@ -9267,10 +9272,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="73" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B103" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C103" s="20" t="s">
         <v>24</v>
@@ -9278,10 +9283,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="73" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B104" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C104" s="20" t="s">
         <v>24</v>
@@ -9289,10 +9294,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="73" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B105" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C105" s="20" t="s">
         <v>24</v>
@@ -9300,10 +9305,10 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="73" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B106" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C106" s="20" t="s">
         <v>24</v>
@@ -9311,10 +9316,10 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="73" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B107" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C107" s="20" t="s">
         <v>24</v>
@@ -9322,10 +9327,10 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="73" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B108" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C108" s="20" t="s">
         <v>24</v>
@@ -9333,10 +9338,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="73" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B109" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C109" s="20" t="s">
         <v>24</v>
@@ -9344,10 +9349,10 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="73" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B110" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C110" s="20" t="s">
         <v>24</v>
@@ -9355,10 +9360,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="73" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B111" s="72" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C111" s="20" t="s">
         <v>24</v>
@@ -9366,10 +9371,10 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="73" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B112" s="73" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C112" s="20" t="s">
         <v>24</v>
@@ -9377,10 +9382,10 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="73" t="s">
+        <v>827</v>
+      </c>
+      <c r="B113" s="73" t="s">
         <v>828</v>
-      </c>
-      <c r="B113" s="73" t="s">
-        <v>829</v>
       </c>
       <c r="C113" s="20" t="s">
         <v>24</v>
@@ -9388,10 +9393,10 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="73" t="s">
+        <v>829</v>
+      </c>
+      <c r="B114" s="73" t="s">
         <v>830</v>
-      </c>
-      <c r="B114" s="73" t="s">
-        <v>831</v>
       </c>
       <c r="C114" s="20" t="s">
         <v>24</v>
@@ -9399,10 +9404,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="73" t="s">
+        <v>831</v>
+      </c>
+      <c r="B115" s="73" t="s">
         <v>832</v>
-      </c>
-      <c r="B115" s="73" t="s">
-        <v>833</v>
       </c>
       <c r="C115" s="20" t="s">
         <v>24</v>
@@ -9410,10 +9415,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="73" t="s">
+        <v>833</v>
+      </c>
+      <c r="B116" s="73" t="s">
         <v>834</v>
-      </c>
-      <c r="B116" s="73" t="s">
-        <v>835</v>
       </c>
       <c r="C116" s="20" t="s">
         <v>24</v>
@@ -9421,10 +9426,10 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="73" t="s">
+        <v>835</v>
+      </c>
+      <c r="B117" s="73" t="s">
         <v>836</v>
-      </c>
-      <c r="B117" s="73" t="s">
-        <v>837</v>
       </c>
       <c r="C117" s="20" t="s">
         <v>24</v>
@@ -9432,10 +9437,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="73" t="s">
+        <v>837</v>
+      </c>
+      <c r="B118" s="73" t="s">
         <v>838</v>
-      </c>
-      <c r="B118" s="73" t="s">
-        <v>839</v>
       </c>
       <c r="C118" s="20" t="s">
         <v>24</v>
@@ -9443,10 +9448,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="73" t="s">
+        <v>839</v>
+      </c>
+      <c r="B119" s="73" t="s">
         <v>840</v>
-      </c>
-      <c r="B119" s="73" t="s">
-        <v>841</v>
       </c>
       <c r="C119" s="20" t="s">
         <v>24</v>
@@ -9454,7 +9459,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="73" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B120" s="74"/>
       <c r="C120" s="20" t="s">
@@ -9463,7 +9468,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="73" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B121" s="74"/>
       <c r="C121" s="20" t="s">
@@ -9472,7 +9477,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="73" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B122" s="74"/>
       <c r="C122" s="20" t="s">
@@ -9481,7 +9486,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="73" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B123" s="74"/>
       <c r="C123" s="20" t="s">
@@ -9609,10 +9614,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="24" t="s">
+        <v>750</v>
+      </c>
+      <c r="B135" s="36" t="s">
         <v>751</v>
-      </c>
-      <c r="B135" s="36" t="s">
-        <v>752</v>
       </c>
       <c r="C135" s="29" t="s">
         <v>24</v>
@@ -9620,10 +9625,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="22" t="s">
+        <v>758</v>
+      </c>
+      <c r="B136" s="20" t="s">
         <v>759</v>
-      </c>
-      <c r="B136" s="20" t="s">
-        <v>760</v>
       </c>
       <c r="C136" s="29" t="s">
         <v>24</v>
@@ -9631,10 +9636,10 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="22" t="s">
+        <v>765</v>
+      </c>
+      <c r="B137" s="20" t="s">
         <v>766</v>
-      </c>
-      <c r="B137" s="20" t="s">
-        <v>767</v>
       </c>
       <c r="C137" s="29" t="s">
         <v>24</v>
@@ -9726,10 +9731,10 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="22" t="s">
+        <v>747</v>
+      </c>
+      <c r="B146" s="20" t="s">
         <v>748</v>
-      </c>
-      <c r="B146" s="20" t="s">
-        <v>749</v>
       </c>
       <c r="C146" s="35" t="s">
         <v>24</v>
@@ -9737,10 +9742,10 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="B147" s="20" t="s">
         <v>755</v>
-      </c>
-      <c r="B147" s="20" t="s">
-        <v>756</v>
       </c>
       <c r="C147" s="35" t="s">
         <v>24</v>
@@ -9748,10 +9753,10 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="B148" s="20" t="s">
         <v>764</v>
-      </c>
-      <c r="B148" s="20" t="s">
-        <v>765</v>
       </c>
       <c r="C148" s="35" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Updated test data commit User ID: Gowtham
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="16" activeTab="16"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -5351,7 +5351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -7004,8 +7004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7042,7 +7042,7 @@
         <v>669</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>682</v>
+        <v>774</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -7055,7 +7055,7 @@
         <v>671</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>682</v>
+        <v>774</v>
       </c>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
@@ -7068,7 +7068,7 @@
         <v>673</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>682</v>
+        <v>774</v>
       </c>
       <c r="D4" s="57" t="s">
         <v>737</v>
@@ -7085,7 +7085,7 @@
         <v>675</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>682</v>
+        <v>774</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>

</xml_diff>

<commit_message>
Disbursement maker checker drawdown and payment details code commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="26" activeTab="29"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="26" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -36,16 +36,17 @@
     <sheet name="AL_Off_facilityDetails_610" sheetId="30" r:id="rId27"/>
     <sheet name="AL_ADE_CustDetValues_610_" sheetId="31" r:id="rId28"/>
     <sheet name="AL_ADE_DocDetValues_610" sheetId="32" r:id="rId29"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId30"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId31"/>
-    <sheet name="Sheet1" sheetId="33" r:id="rId32"/>
+    <sheet name="DSBMKRCHR_PaymentSchedTestData" sheetId="34" r:id="rId30"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId31"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId32"/>
+    <sheet name="Sheet1" sheetId="33" r:id="rId33"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="871">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2616,6 +2617,48 @@
   </si>
   <si>
     <t>1069</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_01</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_AL_PS_DSP_02</t>
+  </si>
+  <si>
+    <t>AT_AL_PS_DSP_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_04</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DD_05</t>
+  </si>
+  <si>
+    <t>Payment_type</t>
+  </si>
+  <si>
+    <t>payee</t>
+  </si>
+  <si>
+    <t>planned_scheduled_amount</t>
+  </si>
+  <si>
+    <t>schedule_notes</t>
+  </si>
+  <si>
+    <t>12000</t>
   </si>
 </sst>
 </file>
@@ -8166,10 +8209,79 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>866</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>867</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>868</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>859</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9511,6 +9623,80 @@
         <v>762</v>
       </c>
       <c r="C121" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="22" t="s">
+        <v>857</v>
+      </c>
+      <c r="B122" s="18"/>
+      <c r="C122" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="B123" s="20" t="s">
+        <v>859</v>
+      </c>
+      <c r="C123" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="B124" s="18"/>
+      <c r="C124" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="B125" s="18"/>
+      <c r="C125" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="B126" s="18"/>
+      <c r="C126" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B127" s="18"/>
+      <c r="C127" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="B128" s="18"/>
+      <c r="C128" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="B129" s="18"/>
+      <c r="C129" s="35" t="s">
         <v>24</v>
       </c>
     </row>
@@ -9541,7 +9727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -9682,7 +9868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>

</xml_diff>

<commit_message>
AutoLoan AppDataEntry Address Details, AutoLoan AppData Entry Asset Details, AutoLoan Offering Customer Details features Commit User : Ramya
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="26" activeTab="30"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="30" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -37,16 +37,18 @@
     <sheet name="AL_ADE_CustDetValues_610_" sheetId="31" r:id="rId28"/>
     <sheet name="AL_ADE_DocDetValues_610" sheetId="32" r:id="rId29"/>
     <sheet name="DSBMKRCHR_PaymentSchedTestData" sheetId="34" r:id="rId30"/>
-    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId31"/>
-    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId32"/>
-    <sheet name="Sheet1" sheetId="33" r:id="rId33"/>
+    <sheet name="AutoL_AppDataEn_AddressDetail" sheetId="35" r:id="rId31"/>
+    <sheet name="AppDataEn_AL_AssetD" sheetId="36" r:id="rId32"/>
+    <sheet name="AutoLoanExecution" sheetId="2" r:id="rId33"/>
+    <sheet name="DisbursmentMakerExecution" sheetId="11" r:id="rId34"/>
+    <sheet name="Sheet1" sheetId="33" r:id="rId35"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="994">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2659,6 +2661,375 @@
   </si>
   <si>
     <t>12000</t>
+  </si>
+  <si>
+    <t>Address Type</t>
+  </si>
+  <si>
+    <t>Address status</t>
+  </si>
+  <si>
+    <t>residential_or_ocupency_status</t>
+  </si>
+  <si>
+    <t>location_category</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>AddressLine2</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>provience_id</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>district_name</t>
+  </si>
+  <si>
+    <t>zip_code</t>
+  </si>
+  <si>
+    <t>po_box_number</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>duration_on_stay</t>
+  </si>
+  <si>
+    <t>latitude_details</t>
+  </si>
+  <si>
+    <t>longitude_details</t>
+  </si>
+  <si>
+    <t>land_mark</t>
+  </si>
+  <si>
+    <t>occupancy_date</t>
+  </si>
+  <si>
+    <t>land_lord_name</t>
+  </si>
+  <si>
+    <t>land_lord_mobile_number</t>
+  </si>
+  <si>
+    <t>rent_amount</t>
+  </si>
+  <si>
+    <t>frequency_of_rent</t>
+  </si>
+  <si>
+    <t>characterInput</t>
+  </si>
+  <si>
+    <t>negative_numeric</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_01</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_01_D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial rent </t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Maharastra</t>
+  </si>
+  <si>
+    <t>BHANDARA</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>9632587410</t>
+  </si>
+  <si>
+    <t>9874563210</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_09</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_09_D1</t>
+  </si>
+  <si>
+    <t>@#$%^</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_02</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_03</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_04</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_05</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_06</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_07</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_08</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_10</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_11</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_12</t>
+  </si>
+  <si>
+    <t>AT_AU_AD_13</t>
+  </si>
+  <si>
+    <t>0323</t>
+  </si>
+  <si>
+    <t>userType18</t>
+  </si>
+  <si>
+    <t>AppDataEntry-AddressDetails</t>
+  </si>
+  <si>
+    <t>asset_manufacture</t>
+  </si>
+  <si>
+    <t>asset_model</t>
+  </si>
+  <si>
+    <t>asset_model_type</t>
+  </si>
+  <si>
+    <t>year of manufacture</t>
+  </si>
+  <si>
+    <t>asset_condition</t>
+  </si>
+  <si>
+    <t>asset_color</t>
+  </si>
+  <si>
+    <t>drivetrain</t>
+  </si>
+  <si>
+    <t>number_of_cylinder</t>
+  </si>
+  <si>
+    <t>volume_of_engine</t>
+  </si>
+  <si>
+    <t>no_of_units</t>
+  </si>
+  <si>
+    <t>chasis_number</t>
+  </si>
+  <si>
+    <t>plate_number</t>
+  </si>
+  <si>
+    <t>plate_number_arabic</t>
+  </si>
+  <si>
+    <t>asset_dealer_dropdown</t>
+  </si>
+  <si>
+    <t>agent_name</t>
+  </si>
+  <si>
+    <t>agent_email_id</t>
+  </si>
+  <si>
+    <t>agent_mobile_number</t>
+  </si>
+  <si>
+    <t>down_payment</t>
+  </si>
+  <si>
+    <t>residual_value</t>
+  </si>
+  <si>
+    <t>green_card_number</t>
+  </si>
+  <si>
+    <t>weight_in_tons</t>
+  </si>
+  <si>
+    <t>mileage</t>
+  </si>
+  <si>
+    <t>country_of_manufacture</t>
+  </si>
+  <si>
+    <t>asset_agreed_fulfilment_location</t>
+  </si>
+  <si>
+    <t>location_of_signing_the_agreement</t>
+  </si>
+  <si>
+    <t>asset_received_location</t>
+  </si>
+  <si>
+    <t>Character_input</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_01_D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tata Motors </t>
+  </si>
+  <si>
+    <t>TATA Harrier</t>
+  </si>
+  <si>
+    <t>1.4L, AT, SR, Remote</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Four Wheeler</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>TN23 1234</t>
+  </si>
+  <si>
+    <t>أمروتا</t>
+  </si>
+  <si>
+    <t>Dealer 1</t>
+  </si>
+  <si>
+    <t>abc098@gmail.com</t>
+  </si>
+  <si>
+    <t>9856324109</t>
+  </si>
+  <si>
+    <t>10000000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>NAGPUR</t>
+  </si>
+  <si>
+    <t>-0987</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_04</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_05</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_06</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_07</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_08</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_09</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_10</t>
+  </si>
+  <si>
+    <t>AT_AL_ASD_11</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_01_D1</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_04</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_05</t>
+  </si>
+  <si>
+    <t>AT_AL_OFF_CD_06</t>
+  </si>
+  <si>
+    <t>matching_value</t>
+  </si>
+  <si>
+    <t>mismatching_value</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>mismatch</t>
   </si>
 </sst>
 </file>
@@ -2668,7 +3039,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2788,6 +3159,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3025,7 +3408,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -3042,8 +3425,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -3160,8 +3544,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="15" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="9"/>
     <cellStyle name="Excel_20_Built-in_20_Hyperlink" xfId="4"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="2"/>
     <cellStyle name="Heading" xfId="5"/>
@@ -3172,7 +3563,7 @@
     <cellStyle name="Result" xfId="7"/>
     <cellStyle name="Result2" xfId="8"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3182,6 +3573,198 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3559,10 +4142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3760,6 +4343,20 @@
         <v>767</v>
       </c>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="37" t="s">
+        <v>924</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>923</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>925</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -3772,8 +4369,12 @@
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="C12" r:id="rId9"/>
     <hyperlink ref="C13" r:id="rId10"/>
+    <hyperlink ref="C14" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B14" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -5075,8 +5676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5345,7 +5946,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7094,16 +7695,16 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7128,23 +7729,23 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>666</v>
+        <v>984</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>667</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>772</v>
+        <v>983</v>
+      </c>
+      <c r="C2" s="43">
+        <v>4006</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>772</v>
@@ -7154,10 +7755,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="22" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>772</v>
@@ -7171,16 +7772,27 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="22" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>772</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="22" t="s">
+        <v>672</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>673</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>772</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8211,9 +8823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8278,10 +8888,544 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="28" max="28" width="20.7109375" customWidth="1"/>
+    <col min="30" max="30" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>875</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="AC1" s="83" t="s">
+        <v>990</v>
+      </c>
+      <c r="AD1" s="83" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
+      <c r="A2" s="41" t="s">
+        <v>895</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>896</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5231</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="N2" s="7">
+        <v>987456</v>
+      </c>
+      <c r="O2" s="7">
+        <v>974121</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>20</v>
+      </c>
+      <c r="R2" s="7">
+        <v>101010</v>
+      </c>
+      <c r="S2" s="7">
+        <v>101010</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="U2" s="7">
+        <v>36779</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="X2" s="7">
+        <v>10000</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7">
+        <v>-123</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="41" t="s">
+        <v>908</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>909</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5231</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="N3" s="7">
+        <v>987456</v>
+      </c>
+      <c r="O3" s="7">
+        <v>974121</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>20</v>
+      </c>
+      <c r="R3" s="7">
+        <v>101010</v>
+      </c>
+      <c r="S3" s="7">
+        <v>101010</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="U3" s="7">
+        <v>36779</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="X3" s="7">
+        <v>10000</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>-123</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="P2:P3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="15.75">
+      <c r="A1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>926</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>927</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>928</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>929</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>930</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>931</v>
+      </c>
+      <c r="J1" s="78" t="s">
+        <v>932</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>933</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>934</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>935</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>936</v>
+      </c>
+      <c r="O1" s="78" t="s">
+        <v>937</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>938</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>939</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>940</v>
+      </c>
+      <c r="S1" s="78" t="s">
+        <v>941</v>
+      </c>
+      <c r="T1" s="78" t="s">
+        <v>942</v>
+      </c>
+      <c r="U1" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>943</v>
+      </c>
+      <c r="W1" s="78" t="s">
+        <v>944</v>
+      </c>
+      <c r="X1" s="78" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y1" s="78" t="s">
+        <v>946</v>
+      </c>
+      <c r="Z1" s="78" t="s">
+        <v>947</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>948</v>
+      </c>
+      <c r="AB1" s="78" t="s">
+        <v>949</v>
+      </c>
+      <c r="AC1" s="78" t="s">
+        <v>950</v>
+      </c>
+      <c r="AD1" s="78" t="s">
+        <v>951</v>
+      </c>
+      <c r="AE1" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF1" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH1" s="78" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15.75">
+      <c r="A2" s="79" t="s">
+        <v>953</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>954</v>
+      </c>
+      <c r="C2">
+        <v>4138</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>955</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>956</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>957</v>
+      </c>
+      <c r="G2" s="81">
+        <v>36779</v>
+      </c>
+      <c r="H2" s="78" t="s">
+        <v>958</v>
+      </c>
+      <c r="I2" s="78" t="s">
+        <v>959</v>
+      </c>
+      <c r="J2" s="78" t="s">
+        <v>960</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" s="78" t="s">
+        <v>961</v>
+      </c>
+      <c r="O2" s="78" t="s">
+        <v>962</v>
+      </c>
+      <c r="P2" s="78" t="s">
+        <v>963</v>
+      </c>
+      <c r="Q2" s="78" t="s">
+        <v>964</v>
+      </c>
+      <c r="R2" s="78" t="s">
+        <v>384</v>
+      </c>
+      <c r="S2" s="78" t="s">
+        <v>965</v>
+      </c>
+      <c r="T2" s="82" t="s">
+        <v>966</v>
+      </c>
+      <c r="U2" s="78" t="s">
+        <v>967</v>
+      </c>
+      <c r="V2" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="W2" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="X2" s="78" t="s">
+        <v>968</v>
+      </c>
+      <c r="Y2" s="78" t="s">
+        <v>968</v>
+      </c>
+      <c r="Z2" s="78" t="s">
+        <v>969</v>
+      </c>
+      <c r="AA2" s="78" t="s">
+        <v>542</v>
+      </c>
+      <c r="AB2" s="78" t="s">
+        <v>970</v>
+      </c>
+      <c r="AC2" s="78" t="s">
+        <v>970</v>
+      </c>
+      <c r="AD2" s="78" t="s">
+        <v>970</v>
+      </c>
+      <c r="AE2" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF2" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="78" t="s">
+        <v>971</v>
+      </c>
+      <c r="AH2" s="78" t="s">
+        <v>972</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="AF2" r:id="rId2" location="$"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="K2:N2 T2:Z2 AG2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H159"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8750,110 +9894,110 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="80" t="s">
+        <v>984</v>
+      </c>
+      <c r="B41" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="80" t="s">
+        <v>985</v>
+      </c>
+      <c r="B42" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="80" t="s">
+        <v>987</v>
+      </c>
+      <c r="B44" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="80" t="s">
+        <v>988</v>
+      </c>
+      <c r="B45" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="80" t="s">
+        <v>989</v>
+      </c>
+      <c r="B46" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="22" t="s">
         <v>666</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B47" s="22" t="s">
         <v>667</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="22" t="s">
+      <c r="C47" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
         <v>668</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B48" s="22" t="s">
         <v>669</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="22" t="s">
+      <c r="C48" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="22" t="s">
         <v>670</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B49" s="22" t="s">
         <v>671</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="22" t="s">
+      <c r="C49" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="22" t="s">
         <v>672</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B50" s="22" t="s">
         <v>673</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="51" t="s">
-        <v>530</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="51" t="s">
-        <v>532</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="51" t="s">
-        <v>536</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>537</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="51" t="s">
-        <v>545</v>
-      </c>
-      <c r="B48" s="50" t="s">
-        <v>537</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="51" t="s">
-        <v>546</v>
-      </c>
-      <c r="B49" s="50" t="s">
-        <v>547</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="51" t="s">
-        <v>548</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>549</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>24</v>
@@ -8861,10 +10005,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="51" t="s">
-        <v>550</v>
-      </c>
-      <c r="B51" s="50" t="s">
-        <v>551</v>
+        <v>530</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>531</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>24</v>
@@ -8872,10 +10016,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="51" t="s">
-        <v>552</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>553</v>
+        <v>532</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>531</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>24</v>
@@ -8883,10 +10027,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="51" t="s">
-        <v>522</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>523</v>
+        <v>536</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>537</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>24</v>
@@ -8894,10 +10038,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="51" t="s">
-        <v>556</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>523</v>
+        <v>545</v>
+      </c>
+      <c r="B54" s="50" t="s">
+        <v>537</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>24</v>
@@ -8905,10 +10049,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="51" t="s">
-        <v>557</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>523</v>
+        <v>546</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>547</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>24</v>
@@ -8916,10 +10060,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="51" t="s">
-        <v>558</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>523</v>
+        <v>548</v>
+      </c>
+      <c r="B56" s="50" t="s">
+        <v>549</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>24</v>
@@ -8927,10 +10071,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="51" t="s">
-        <v>559</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>523</v>
+        <v>550</v>
+      </c>
+      <c r="B57" s="50" t="s">
+        <v>551</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>24</v>
@@ -8938,10 +10082,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="51" t="s">
-        <v>560</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>523</v>
+        <v>552</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>553</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>24</v>
@@ -8949,7 +10093,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="51" t="s">
-        <v>561</v>
+        <v>522</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>523</v>
@@ -8960,7 +10104,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="51" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="B60" s="22" t="s">
         <v>523</v>
@@ -8971,10 +10115,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="51" t="s">
-        <v>592</v>
+        <v>557</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>24</v>
@@ -8982,10 +10126,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="51" t="s">
-        <v>612</v>
+        <v>558</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>24</v>
@@ -8993,10 +10137,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="51" t="s">
-        <v>613</v>
+        <v>559</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>24</v>
@@ -9004,10 +10148,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="51" t="s">
-        <v>614</v>
+        <v>560</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>24</v>
@@ -9015,10 +10159,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="51" t="s">
-        <v>615</v>
+        <v>561</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C65" s="20" t="s">
         <v>24</v>
@@ -9026,10 +10170,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="51" t="s">
-        <v>616</v>
+        <v>562</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>24</v>
@@ -9037,7 +10181,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="51" t="s">
-        <v>617</v>
+        <v>592</v>
       </c>
       <c r="B67" s="22" t="s">
         <v>593</v>
@@ -9048,7 +10192,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="51" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>593</v>
@@ -9059,7 +10203,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="51" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>593</v>
@@ -9070,7 +10214,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="51" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B70" s="22" t="s">
         <v>593</v>
@@ -9081,7 +10225,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="51" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>593</v>
@@ -9092,76 +10236,76 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="51" t="s">
+        <v>616</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="51" t="s">
+        <v>617</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="51" t="s">
+        <v>621</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="51" t="s">
         <v>554</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B78" s="50" t="s">
         <v>555</v>
-      </c>
-      <c r="C72" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="22" t="s">
-        <v>387</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>388</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="22" t="s">
-        <v>392</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="22" t="s">
-        <v>397</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="22" t="s">
-        <v>404</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>405</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>24</v>
@@ -9169,10 +10313,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="22" t="s">
-        <v>406</v>
+        <v>371</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>407</v>
+        <v>372</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>24</v>
@@ -9180,10 +10324,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="22" t="s">
-        <v>408</v>
+        <v>376</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>409</v>
+        <v>377</v>
       </c>
       <c r="C80" s="20" t="s">
         <v>24</v>
@@ -9191,10 +10335,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="22" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="C81" s="20" t="s">
         <v>24</v>
@@ -9202,10 +10346,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="22" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="C82" s="20" t="s">
         <v>24</v>
@@ -9213,10 +10357,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="22" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C83" s="20" t="s">
         <v>24</v>
@@ -9224,76 +10368,76 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="C88" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="22" t="s">
         <v>417</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B90" s="22" t="s">
         <v>418</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="73" t="s">
-        <v>808</v>
-      </c>
-      <c r="B85" s="73" t="s">
-        <v>824</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="73" t="s">
-        <v>825</v>
-      </c>
-      <c r="B86" s="73" t="s">
-        <v>826</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="73" t="s">
-        <v>827</v>
-      </c>
-      <c r="B87" s="73" t="s">
-        <v>828</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="73" t="s">
-        <v>829</v>
-      </c>
-      <c r="B88" s="73" t="s">
-        <v>830</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="73" t="s">
-        <v>831</v>
-      </c>
-      <c r="B89" s="73" t="s">
-        <v>832</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="73" t="s">
-        <v>833</v>
-      </c>
-      <c r="B90" s="73" t="s">
-        <v>834</v>
       </c>
       <c r="C90" s="20" t="s">
         <v>24</v>
@@ -9301,10 +10445,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="73" t="s">
-        <v>835</v>
+        <v>808</v>
       </c>
       <c r="B91" s="73" t="s">
-        <v>836</v>
+        <v>824</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>24</v>
@@ -9312,10 +10456,10 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="73" t="s">
-        <v>837</v>
+        <v>825</v>
       </c>
       <c r="B92" s="73" t="s">
-        <v>838</v>
+        <v>826</v>
       </c>
       <c r="C92" s="20" t="s">
         <v>24</v>
@@ -9323,282 +10467,284 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="73" t="s">
-        <v>770</v>
-      </c>
-      <c r="B93" s="74"/>
+        <v>827</v>
+      </c>
+      <c r="B93" s="73" t="s">
+        <v>828</v>
+      </c>
       <c r="C93" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="73" t="s">
-        <v>839</v>
-      </c>
-      <c r="B94" s="74"/>
+        <v>829</v>
+      </c>
+      <c r="B94" s="73" t="s">
+        <v>830</v>
+      </c>
       <c r="C94" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="73" t="s">
-        <v>840</v>
-      </c>
-      <c r="B95" s="74"/>
+        <v>831</v>
+      </c>
+      <c r="B95" s="73" t="s">
+        <v>832</v>
+      </c>
       <c r="C95" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="73" t="s">
+        <v>833</v>
+      </c>
+      <c r="B96" s="73" t="s">
+        <v>834</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="73" t="s">
+        <v>835</v>
+      </c>
+      <c r="B97" s="73" t="s">
+        <v>836</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="73" t="s">
+        <v>837</v>
+      </c>
+      <c r="B98" s="73" t="s">
+        <v>838</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="73" t="s">
+        <v>770</v>
+      </c>
+      <c r="B99" s="74"/>
+      <c r="C99" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="73" t="s">
+        <v>839</v>
+      </c>
+      <c r="B100" s="74"/>
+      <c r="C100" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="73" t="s">
+        <v>840</v>
+      </c>
+      <c r="B101" s="74"/>
+      <c r="C101" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="73" t="s">
         <v>841</v>
       </c>
-      <c r="B96" s="74"/>
-      <c r="C96" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="75" t="s">
+      <c r="B102" s="74"/>
+      <c r="C102" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="75" t="s">
         <v>326</v>
       </c>
-      <c r="B97" s="76" t="s">
+      <c r="B103" s="76" t="s">
         <v>327</v>
       </c>
-      <c r="C97" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="41" t="s">
+      <c r="C103" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="B98" s="22" t="s">
+      <c r="B104" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="C98" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="41" t="s">
+      <c r="C104" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B105" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C99" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="41" t="s">
+      <c r="C105" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="41" t="s">
         <v>335</v>
       </c>
-      <c r="B100" s="22" t="s">
+      <c r="B106" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="C100" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="41" t="s">
+      <c r="C106" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="41" t="s">
         <v>347</v>
       </c>
-      <c r="B101" s="22" t="s">
+      <c r="B107" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="C101" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="41" t="s">
+      <c r="C107" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="41" t="s">
         <v>338</v>
       </c>
-      <c r="B102" s="22" t="s">
+      <c r="B108" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="C102" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="B103" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B104" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B105" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B106" s="18"/>
-      <c r="C106" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C107" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="24" t="s">
-        <v>748</v>
-      </c>
-      <c r="B108" s="36" t="s">
-        <v>749</v>
-      </c>
-      <c r="C108" s="29" t="s">
+      <c r="C108" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="22" t="s">
-        <v>756</v>
+        <v>263</v>
       </c>
       <c r="B109" s="20" t="s">
-        <v>757</v>
-      </c>
-      <c r="C109" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="C109" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="22" t="s">
-        <v>763</v>
+        <v>265</v>
       </c>
       <c r="B110" s="20" t="s">
-        <v>764</v>
-      </c>
-      <c r="C110" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C110" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C111" s="29" t="s">
+      <c r="A111" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C111" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="B112" s="33"/>
-      <c r="C112" s="34" t="s">
+      <c r="A112" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B112" s="18"/>
+      <c r="C112" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="C113" s="35" t="s">
+      <c r="A113" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C113" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="B114" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C114" s="35" t="s">
+      <c r="A114" s="24" t="s">
+        <v>748</v>
+      </c>
+      <c r="B114" s="36" t="s">
+        <v>749</v>
+      </c>
+      <c r="C114" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C115" s="35" t="s">
+        <v>756</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>757</v>
+      </c>
+      <c r="C115" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="B116" s="18"/>
-      <c r="C116" s="35" t="s">
+        <v>763</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>764</v>
+      </c>
+      <c r="C116" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="B117" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="C117" s="35" t="s">
+      <c r="A117" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C117" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C118" s="68" t="s">
+      <c r="A118" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B118" s="33"/>
+      <c r="C118" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="22" t="s">
-        <v>745</v>
+        <v>284</v>
       </c>
       <c r="B119" s="20" t="s">
-        <v>746</v>
+        <v>285</v>
       </c>
       <c r="C119" s="35" t="s">
         <v>24</v>
@@ -9606,10 +10752,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="22" t="s">
-        <v>752</v>
+        <v>282</v>
       </c>
       <c r="B120" s="20" t="s">
-        <v>753</v>
+        <v>283</v>
       </c>
       <c r="C120" s="35" t="s">
         <v>24</v>
@@ -9617,10 +10763,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="22" t="s">
-        <v>761</v>
-      </c>
-      <c r="B121" s="20" t="s">
-        <v>762</v>
+        <v>289</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>290</v>
       </c>
       <c r="C121" s="35" t="s">
         <v>24</v>
@@ -9628,7 +10774,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="22" t="s">
-        <v>857</v>
+        <v>294</v>
       </c>
       <c r="B122" s="18"/>
       <c r="C122" s="35" t="s">
@@ -9637,54 +10783,62 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="22" t="s">
-        <v>858</v>
+        <v>295</v>
       </c>
       <c r="B123" s="20" t="s">
-        <v>859</v>
+        <v>296</v>
       </c>
       <c r="C123" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="22" t="s">
-        <v>860</v>
-      </c>
-      <c r="B124" s="18"/>
-      <c r="C124" s="35" t="s">
+      <c r="A124" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C124" s="68" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="22" t="s">
-        <v>861</v>
-      </c>
-      <c r="B125" s="18"/>
+        <v>745</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>746</v>
+      </c>
       <c r="C125" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="B126" s="18"/>
+        <v>752</v>
+      </c>
+      <c r="B126" s="20" t="s">
+        <v>753</v>
+      </c>
       <c r="C126" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="22" t="s">
-        <v>863</v>
-      </c>
-      <c r="B127" s="18"/>
+        <v>761</v>
+      </c>
+      <c r="B127" s="20" t="s">
+        <v>762</v>
+      </c>
       <c r="C127" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="22" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="B128" s="18"/>
       <c r="C128" s="35" t="s">
@@ -9693,32 +10847,410 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="B129" s="20" t="s">
+        <v>859</v>
+      </c>
+      <c r="C129" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="B130" s="18"/>
+      <c r="C130" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="B131" s="18"/>
+      <c r="C131" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="B132" s="18"/>
+      <c r="C132" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B133" s="18"/>
+      <c r="C133" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="B134" s="18"/>
+      <c r="C134" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="22" t="s">
         <v>865</v>
       </c>
-      <c r="B129" s="18"/>
-      <c r="C129" s="35" t="s">
+      <c r="B135" s="18"/>
+      <c r="C135" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="80" t="s">
+        <v>895</v>
+      </c>
+      <c r="B136" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="80" t="s">
+        <v>912</v>
+      </c>
+      <c r="B137" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C137" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="80" t="s">
+        <v>913</v>
+      </c>
+      <c r="B138" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="80" t="s">
+        <v>914</v>
+      </c>
+      <c r="B139" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="80" t="s">
+        <v>915</v>
+      </c>
+      <c r="B140" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="80" t="s">
+        <v>916</v>
+      </c>
+      <c r="B141" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C141" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="80" t="s">
+        <v>917</v>
+      </c>
+      <c r="B142" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C142" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="80" t="s">
+        <v>918</v>
+      </c>
+      <c r="B143" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="80" t="s">
+        <v>908</v>
+      </c>
+      <c r="B144" s="80" t="s">
+        <v>909</v>
+      </c>
+      <c r="C144" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="80" t="s">
+        <v>919</v>
+      </c>
+      <c r="B145" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="80" t="s">
+        <v>920</v>
+      </c>
+      <c r="B146" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="80" t="s">
+        <v>921</v>
+      </c>
+      <c r="B147" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C147" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="80" t="s">
+        <v>922</v>
+      </c>
+      <c r="B148" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C148" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="80" t="s">
+        <v>953</v>
+      </c>
+      <c r="B149" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C149" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="80" t="s">
+        <v>973</v>
+      </c>
+      <c r="B150" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C150" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="80" t="s">
+        <v>974</v>
+      </c>
+      <c r="B151" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C151" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="80" t="s">
+        <v>975</v>
+      </c>
+      <c r="B152" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C152" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="80" t="s">
+        <v>976</v>
+      </c>
+      <c r="B153" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C153" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="80" t="s">
+        <v>977</v>
+      </c>
+      <c r="B154" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C154" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="80" t="s">
+        <v>978</v>
+      </c>
+      <c r="B155" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C155" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="80" t="s">
+        <v>979</v>
+      </c>
+      <c r="B156" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C156" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="80" t="s">
+        <v>980</v>
+      </c>
+      <c r="B157" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C157" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="80" t="s">
+        <v>981</v>
+      </c>
+      <c r="B158" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C158" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="80" t="s">
+        <v>982</v>
+      </c>
+      <c r="B159" s="80" t="s">
+        <v>954</v>
+      </c>
+      <c r="C159" s="20" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C115">
-    <cfRule type="cellIs" dxfId="7" priority="33" operator="equal">
+  <conditionalFormatting sqref="C2:C121">
+    <cfRule type="cellIs" dxfId="23" priority="53" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85:C96">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C85)))</formula>
+  <conditionalFormatting sqref="C91:C102">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C85)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C136:C148">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C136)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C136)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C137:C148">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C136:C148">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C136:C148">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C149)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C149)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C149)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C149)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C149:C159">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C115">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C136:C159 C2:C121">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9727,7 +11259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -9868,12 +11400,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" activeCellId="3" sqref="A33:XFD33 A34:XFD34 A35:XFD35 A36:XFD36"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12512,7 +14044,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Auto Loan code changes updated execution tracker commited User ID: Anandh
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="30" activeTab="30"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23250" windowHeight="12540" firstSheet="30" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="994">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -3563,7 +3563,79 @@
     <cellStyle name="Result" xfId="7"/>
     <cellStyle name="Result2" xfId="8"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3765,6 +3837,78 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8890,7 +9034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
@@ -9422,10 +9566,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9806,77 +9950,77 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="22" t="s">
-        <v>650</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>651</v>
+      <c r="A33" s="54" t="s">
+        <v>636</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>637</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>653</v>
+      <c r="A34" s="54" t="s">
+        <v>638</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>639</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="22" t="s">
-        <v>654</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>655</v>
+      <c r="A35" s="54" t="s">
+        <v>640</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>641</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>657</v>
+      <c r="A36" s="54" t="s">
+        <v>642</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>643</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="22" t="s">
-        <v>658</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>659</v>
+      <c r="A37" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>645</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>661</v>
+      <c r="A38" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B38" s="54" t="s">
+        <v>647</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>663</v>
+      <c r="A39" s="54" t="s">
+        <v>648</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>649</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>24</v>
@@ -9884,76 +10028,76 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="22" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="80" t="s">
-        <v>984</v>
-      </c>
-      <c r="B41" s="80" t="s">
-        <v>983</v>
+      <c r="A41" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>653</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="80" t="s">
-        <v>985</v>
-      </c>
-      <c r="B42" s="80" t="s">
-        <v>983</v>
+      <c r="A42" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>655</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="80" t="s">
-        <v>986</v>
-      </c>
-      <c r="B43" s="80" t="s">
-        <v>983</v>
+      <c r="A43" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>657</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="80" t="s">
-        <v>987</v>
-      </c>
-      <c r="B44" s="80" t="s">
-        <v>983</v>
+      <c r="A44" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>659</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="80" t="s">
-        <v>988</v>
-      </c>
-      <c r="B45" s="80" t="s">
-        <v>983</v>
+      <c r="A45" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>661</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="80" t="s">
-        <v>989</v>
-      </c>
-      <c r="B46" s="80" t="s">
-        <v>983</v>
+      <c r="A46" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>663</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>24</v>
@@ -9961,120 +10105,120 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>665</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="80" t="s">
+        <v>984</v>
+      </c>
+      <c r="B48" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="80" t="s">
+        <v>985</v>
+      </c>
+      <c r="B49" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="80" t="s">
+        <v>986</v>
+      </c>
+      <c r="B50" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="80" t="s">
+        <v>987</v>
+      </c>
+      <c r="B51" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="80" t="s">
+        <v>988</v>
+      </c>
+      <c r="B52" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="80" t="s">
+        <v>989</v>
+      </c>
+      <c r="B53" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="22" t="s">
         <v>666</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B54" s="22" t="s">
         <v>667</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="22" t="s">
+      <c r="C54" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="22" t="s">
         <v>668</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B55" s="22" t="s">
         <v>669</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="22" t="s">
+      <c r="C55" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="22" t="s">
         <v>670</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B56" s="22" t="s">
         <v>671</v>
       </c>
-      <c r="C49" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="22" t="s">
+      <c r="C56" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="22" t="s">
         <v>672</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B57" s="22" t="s">
         <v>673</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="51" t="s">
-        <v>530</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="51" t="s">
-        <v>532</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="51" t="s">
-        <v>536</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>537</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="51" t="s">
-        <v>545</v>
-      </c>
-      <c r="B54" s="50" t="s">
-        <v>537</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="51" t="s">
-        <v>546</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>547</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="51" t="s">
-        <v>548</v>
-      </c>
-      <c r="B56" s="50" t="s">
-        <v>549</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="51" t="s">
-        <v>550</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>551</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>24</v>
@@ -10082,10 +10226,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="51" t="s">
-        <v>552</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>553</v>
+        <v>530</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>531</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>24</v>
@@ -10093,10 +10237,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="51" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>24</v>
@@ -10104,10 +10248,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="51" t="s">
-        <v>556</v>
-      </c>
-      <c r="B60" s="22" t="s">
-        <v>523</v>
+        <v>536</v>
+      </c>
+      <c r="B60" s="50" t="s">
+        <v>537</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>24</v>
@@ -10115,10 +10259,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="51" t="s">
-        <v>557</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>523</v>
+        <v>545</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>537</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>24</v>
@@ -10126,10 +10270,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="51" t="s">
-        <v>558</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>523</v>
+        <v>546</v>
+      </c>
+      <c r="B62" s="50" t="s">
+        <v>547</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>24</v>
@@ -10137,10 +10281,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="51" t="s">
-        <v>559</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>523</v>
+        <v>548</v>
+      </c>
+      <c r="B63" s="50" t="s">
+        <v>549</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>24</v>
@@ -10148,10 +10292,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="51" t="s">
-        <v>560</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>523</v>
+        <v>550</v>
+      </c>
+      <c r="B64" s="50" t="s">
+        <v>551</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>24</v>
@@ -10159,10 +10303,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>523</v>
+        <v>552</v>
+      </c>
+      <c r="B65" s="50" t="s">
+        <v>553</v>
       </c>
       <c r="C65" s="20" t="s">
         <v>24</v>
@@ -10170,7 +10314,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="51" t="s">
-        <v>562</v>
+        <v>522</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>523</v>
@@ -10181,10 +10325,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="51" t="s">
-        <v>592</v>
+        <v>556</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C67" s="20" t="s">
         <v>24</v>
@@ -10192,10 +10336,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="51" t="s">
-        <v>612</v>
+        <v>557</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>24</v>
@@ -10203,10 +10347,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="51" t="s">
-        <v>613</v>
+        <v>558</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C69" s="20" t="s">
         <v>24</v>
@@ -10214,10 +10358,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="51" t="s">
-        <v>614</v>
+        <v>559</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C70" s="20" t="s">
         <v>24</v>
@@ -10225,10 +10369,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="51" t="s">
-        <v>615</v>
+        <v>560</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>24</v>
@@ -10236,10 +10380,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="51" t="s">
-        <v>616</v>
+        <v>561</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>24</v>
@@ -10247,10 +10391,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="51" t="s">
-        <v>617</v>
+        <v>562</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>593</v>
+        <v>523</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>24</v>
@@ -10258,7 +10402,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="51" t="s">
-        <v>618</v>
+        <v>592</v>
       </c>
       <c r="B74" s="22" t="s">
         <v>593</v>
@@ -10269,7 +10413,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="51" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B75" s="22" t="s">
         <v>593</v>
@@ -10280,7 +10424,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="51" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>593</v>
@@ -10291,7 +10435,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="51" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>593</v>
@@ -10302,87 +10446,87 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="51" t="s">
+        <v>615</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="51" t="s">
+        <v>616</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="51" t="s">
+        <v>617</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="51" t="s">
+        <v>621</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="51" t="s">
         <v>554</v>
       </c>
-      <c r="B78" s="50" t="s">
+      <c r="B85" s="50" t="s">
         <v>555</v>
-      </c>
-      <c r="C78" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="22" t="s">
-        <v>371</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="C79" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>377</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="22" t="s">
-        <v>387</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>388</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="22" t="s">
-        <v>392</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="22" t="s">
-        <v>397</v>
-      </c>
-      <c r="B83" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="22" t="s">
-        <v>404</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>405</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="22" t="s">
-        <v>406</v>
-      </c>
-      <c r="B85" s="22" t="s">
-        <v>407</v>
       </c>
       <c r="C85" s="20" t="s">
         <v>24</v>
@@ -10390,10 +10534,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="22" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>409</v>
+        <v>372</v>
       </c>
       <c r="C86" s="20" t="s">
         <v>24</v>
@@ -10401,10 +10545,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="22" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>411</v>
+        <v>377</v>
       </c>
       <c r="C87" s="20" t="s">
         <v>24</v>
@@ -10412,10 +10556,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="22" t="s">
-        <v>412</v>
+        <v>387</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C88" s="20" t="s">
         <v>24</v>
@@ -10423,10 +10567,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="22" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
       <c r="C89" s="20" t="s">
         <v>24</v>
@@ -10434,823 +10578,1144 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>415</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="22" t="s">
         <v>417</v>
       </c>
-      <c r="B90" s="22" t="s">
+      <c r="B97" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="C90" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="73" t="s">
+      <c r="C97" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="22" t="s">
+        <v>438</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="22" t="s">
+        <v>448</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>460</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="B105" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="72" t="s">
+        <v>794</v>
+      </c>
+      <c r="B107" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="73" t="s">
+        <v>814</v>
+      </c>
+      <c r="B108" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="73" t="s">
+        <v>815</v>
+      </c>
+      <c r="B109" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="73" t="s">
+        <v>816</v>
+      </c>
+      <c r="B110" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="73" t="s">
+        <v>817</v>
+      </c>
+      <c r="B111" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C111" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="73" t="s">
+        <v>818</v>
+      </c>
+      <c r="B112" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="73" t="s">
+        <v>819</v>
+      </c>
+      <c r="B113" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C113" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="73" t="s">
+        <v>820</v>
+      </c>
+      <c r="B114" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C114" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="73" t="s">
+        <v>821</v>
+      </c>
+      <c r="B115" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C115" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="73" t="s">
+        <v>822</v>
+      </c>
+      <c r="B116" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="73" t="s">
+        <v>823</v>
+      </c>
+      <c r="B117" s="72" t="s">
+        <v>813</v>
+      </c>
+      <c r="C117" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="73" t="s">
         <v>808</v>
       </c>
-      <c r="B91" s="73" t="s">
+      <c r="B118" s="73" t="s">
         <v>824</v>
       </c>
-      <c r="C91" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="73" t="s">
+      <c r="C118" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="73" t="s">
         <v>825</v>
       </c>
-      <c r="B92" s="73" t="s">
+      <c r="B119" s="73" t="s">
         <v>826</v>
       </c>
-      <c r="C92" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="73" t="s">
+      <c r="C119" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="73" t="s">
         <v>827</v>
       </c>
-      <c r="B93" s="73" t="s">
+      <c r="B120" s="73" t="s">
         <v>828</v>
       </c>
-      <c r="C93" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="73" t="s">
+      <c r="C120" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="73" t="s">
         <v>829</v>
       </c>
-      <c r="B94" s="73" t="s">
+      <c r="B121" s="73" t="s">
         <v>830</v>
       </c>
-      <c r="C94" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="73" t="s">
+      <c r="C121" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="73" t="s">
         <v>831</v>
       </c>
-      <c r="B95" s="73" t="s">
+      <c r="B122" s="73" t="s">
         <v>832</v>
       </c>
-      <c r="C95" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="73" t="s">
+      <c r="C122" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="73" t="s">
         <v>833</v>
       </c>
-      <c r="B96" s="73" t="s">
+      <c r="B123" s="73" t="s">
         <v>834</v>
       </c>
-      <c r="C96" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="73" t="s">
+      <c r="C123" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="73" t="s">
         <v>835</v>
       </c>
-      <c r="B97" s="73" t="s">
+      <c r="B124" s="73" t="s">
         <v>836</v>
       </c>
-      <c r="C97" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="73" t="s">
+      <c r="C124" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="73" t="s">
         <v>837</v>
       </c>
-      <c r="B98" s="73" t="s">
+      <c r="B125" s="73" t="s">
         <v>838</v>
       </c>
-      <c r="C98" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="73" t="s">
+      <c r="C125" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="73" t="s">
         <v>770</v>
       </c>
-      <c r="B99" s="74"/>
-      <c r="C99" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="73" t="s">
+      <c r="B126" s="74"/>
+      <c r="C126" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="73" t="s">
         <v>839</v>
       </c>
-      <c r="B100" s="74"/>
-      <c r="C100" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="73" t="s">
+      <c r="B127" s="74"/>
+      <c r="C127" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="73" t="s">
         <v>840</v>
       </c>
-      <c r="B101" s="74"/>
-      <c r="C101" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="73" t="s">
+      <c r="B128" s="74"/>
+      <c r="C128" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="73" t="s">
         <v>841</v>
       </c>
-      <c r="B102" s="74"/>
-      <c r="C102" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="75" t="s">
+      <c r="B129" s="74"/>
+      <c r="C129" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="75" t="s">
         <v>326</v>
       </c>
-      <c r="B103" s="76" t="s">
+      <c r="B130" s="76" t="s">
         <v>327</v>
       </c>
-      <c r="C103" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="41" t="s">
+      <c r="C130" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="B104" s="22" t="s">
+      <c r="B131" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="C104" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="41" t="s">
+      <c r="C131" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="B132" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C105" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="41" t="s">
+      <c r="C132" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="41" t="s">
         <v>335</v>
       </c>
-      <c r="B106" s="22" t="s">
+      <c r="B133" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="C106" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="41" t="s">
+      <c r="C133" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="41" t="s">
         <v>347</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B134" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="C107" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="41" t="s">
+      <c r="C134" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="41" t="s">
         <v>338</v>
       </c>
-      <c r="B108" s="22" t="s">
+      <c r="B135" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="C108" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="22" t="s">
+      <c r="C135" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="B136" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="C109" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="22" t="s">
+      <c r="C136" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B137" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="C110" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="22" t="s">
+      <c r="C137" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="B111" s="20" t="s">
+      <c r="B138" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="C111" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="22" t="s">
+      <c r="C138" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B112" s="18"/>
-      <c r="C112" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="6" t="s">
+      <c r="B139" s="18"/>
+      <c r="C139" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B140" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C113" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="24" t="s">
+      <c r="C140" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="24" t="s">
         <v>748</v>
       </c>
-      <c r="B114" s="36" t="s">
+      <c r="B141" s="36" t="s">
         <v>749</v>
       </c>
-      <c r="C114" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="22" t="s">
+      <c r="C141" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="22" t="s">
         <v>756</v>
       </c>
-      <c r="B115" s="20" t="s">
+      <c r="B142" s="20" t="s">
         <v>757</v>
       </c>
-      <c r="C115" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="22" t="s">
+      <c r="C142" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="22" t="s">
         <v>763</v>
       </c>
-      <c r="B116" s="20" t="s">
+      <c r="B143" s="20" t="s">
         <v>764</v>
       </c>
-      <c r="C116" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="6" t="s">
+      <c r="C143" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="B144" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C117" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="32" t="s">
+      <c r="C144" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="B118" s="33"/>
-      <c r="C118" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="22" t="s">
+      <c r="B145" s="33"/>
+      <c r="C145" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="B146" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="C119" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="22" t="s">
+      <c r="C146" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="B120" s="20" t="s">
+      <c r="B147" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="C120" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="22" t="s">
+      <c r="C147" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="B148" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C121" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="22" t="s">
+      <c r="C148" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="B122" s="18"/>
-      <c r="C122" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="22" t="s">
+      <c r="B149" s="18"/>
+      <c r="C149" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="B123" s="20" t="s">
+      <c r="B150" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="C123" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="6" t="s">
+      <c r="C150" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B124" s="7" t="s">
+      <c r="B151" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C124" s="68" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="22" t="s">
+      <c r="C151" s="68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="22" t="s">
         <v>745</v>
       </c>
-      <c r="B125" s="20" t="s">
+      <c r="B152" s="20" t="s">
         <v>746</v>
       </c>
-      <c r="C125" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="22" t="s">
+      <c r="C152" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="B153" s="20" t="s">
         <v>753</v>
       </c>
-      <c r="C126" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="22" t="s">
+      <c r="C153" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="22" t="s">
         <v>761</v>
       </c>
-      <c r="B127" s="20" t="s">
+      <c r="B154" s="20" t="s">
         <v>762</v>
       </c>
-      <c r="C127" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="22" t="s">
+      <c r="C154" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="22" t="s">
         <v>857</v>
       </c>
-      <c r="B128" s="18"/>
-      <c r="C128" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="22" t="s">
+      <c r="B155" s="18"/>
+      <c r="C155" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="22" t="s">
         <v>858</v>
       </c>
-      <c r="B129" s="20" t="s">
+      <c r="B156" s="20" t="s">
         <v>859</v>
       </c>
-      <c r="C129" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="22" t="s">
+      <c r="C156" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="22" t="s">
         <v>860</v>
       </c>
-      <c r="B130" s="18"/>
-      <c r="C130" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="22" t="s">
+      <c r="B157" s="18"/>
+      <c r="C157" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="22" t="s">
         <v>861</v>
       </c>
-      <c r="B131" s="18"/>
-      <c r="C131" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="22" t="s">
+      <c r="B158" s="18"/>
+      <c r="C158" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="22" t="s">
         <v>862</v>
       </c>
-      <c r="B132" s="18"/>
-      <c r="C132" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="22" t="s">
+      <c r="B159" s="18"/>
+      <c r="C159" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="22" t="s">
         <v>863</v>
       </c>
-      <c r="B133" s="18"/>
-      <c r="C133" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="22" t="s">
+      <c r="B160" s="18"/>
+      <c r="C160" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="22" t="s">
         <v>864</v>
       </c>
-      <c r="B134" s="18"/>
-      <c r="C134" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="22" t="s">
+      <c r="B161" s="18"/>
+      <c r="C161" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="22" t="s">
         <v>865</v>
       </c>
-      <c r="B135" s="18"/>
-      <c r="C135" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="80" t="s">
+      <c r="B162" s="18"/>
+      <c r="C162" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="80" t="s">
         <v>895</v>
       </c>
-      <c r="B136" s="80" t="s">
+      <c r="B163" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C136" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="80" t="s">
+      <c r="C163" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="80" t="s">
         <v>912</v>
       </c>
-      <c r="B137" s="80" t="s">
+      <c r="B164" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C137" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="80" t="s">
+      <c r="C164" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="80" t="s">
         <v>913</v>
       </c>
-      <c r="B138" s="80" t="s">
+      <c r="B165" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C138" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="80" t="s">
+      <c r="C165" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="80" t="s">
         <v>914</v>
       </c>
-      <c r="B139" s="80" t="s">
+      <c r="B166" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C139" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="80" t="s">
+      <c r="C166" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="80" t="s">
         <v>915</v>
       </c>
-      <c r="B140" s="80" t="s">
+      <c r="B167" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C140" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="80" t="s">
+      <c r="C167" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="80" t="s">
         <v>916</v>
       </c>
-      <c r="B141" s="80" t="s">
+      <c r="B168" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C141" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" s="80" t="s">
+      <c r="C168" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="80" t="s">
         <v>917</v>
       </c>
-      <c r="B142" s="80" t="s">
+      <c r="B169" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C142" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="80" t="s">
+      <c r="C169" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="80" t="s">
         <v>918</v>
       </c>
-      <c r="B143" s="80" t="s">
+      <c r="B170" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C143" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="80" t="s">
+      <c r="C170" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="80" t="s">
         <v>908</v>
       </c>
-      <c r="B144" s="80" t="s">
+      <c r="B171" s="80" t="s">
         <v>909</v>
       </c>
-      <c r="C144" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="80" t="s">
+      <c r="C171" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="80" t="s">
         <v>919</v>
       </c>
-      <c r="B145" s="80" t="s">
+      <c r="B172" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C145" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="80" t="s">
+      <c r="C172" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="80" t="s">
         <v>920</v>
       </c>
-      <c r="B146" s="80" t="s">
+      <c r="B173" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C146" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="80" t="s">
+      <c r="C173" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="80" t="s">
         <v>921</v>
       </c>
-      <c r="B147" s="80" t="s">
+      <c r="B174" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C147" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="80" t="s">
+      <c r="C174" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="80" t="s">
         <v>922</v>
       </c>
-      <c r="B148" s="80" t="s">
+      <c r="B175" s="80" t="s">
         <v>896</v>
       </c>
-      <c r="C148" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" s="80" t="s">
+      <c r="C175" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="80" t="s">
         <v>953</v>
       </c>
-      <c r="B149" s="80" t="s">
+      <c r="B176" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C149" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="80" t="s">
+      <c r="C176" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="80" t="s">
         <v>973</v>
       </c>
-      <c r="B150" s="80" t="s">
+      <c r="B177" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C150" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="80" t="s">
+      <c r="C177" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="80" t="s">
         <v>974</v>
       </c>
-      <c r="B151" s="80" t="s">
+      <c r="B178" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C151" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="80" t="s">
+      <c r="C178" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="80" t="s">
         <v>975</v>
       </c>
-      <c r="B152" s="80" t="s">
+      <c r="B179" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C152" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="80" t="s">
+      <c r="C179" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="80" t="s">
         <v>976</v>
       </c>
-      <c r="B153" s="80" t="s">
+      <c r="B180" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C153" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="80" t="s">
+      <c r="C180" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="80" t="s">
         <v>977</v>
       </c>
-      <c r="B154" s="80" t="s">
+      <c r="B181" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C154" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="80" t="s">
+      <c r="C181" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="80" t="s">
         <v>978</v>
       </c>
-      <c r="B155" s="80" t="s">
+      <c r="B182" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C155" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" s="80" t="s">
+      <c r="C182" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="80" t="s">
         <v>979</v>
       </c>
-      <c r="B156" s="80" t="s">
+      <c r="B183" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C156" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" s="80" t="s">
+      <c r="C183" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="80" t="s">
         <v>980</v>
       </c>
-      <c r="B157" s="80" t="s">
+      <c r="B184" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C157" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158" s="80" t="s">
+      <c r="C184" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="80" t="s">
         <v>981</v>
       </c>
-      <c r="B158" s="80" t="s">
+      <c r="B185" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C158" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="80" t="s">
+      <c r="C185" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="80" t="s">
         <v>982</v>
       </c>
-      <c r="B159" s="80" t="s">
+      <c r="B186" s="80" t="s">
         <v>954</v>
       </c>
-      <c r="C159" s="20" t="s">
+      <c r="C186" s="20" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C121">
-    <cfRule type="cellIs" dxfId="23" priority="53" operator="equal">
+  <conditionalFormatting sqref="C2:C148">
+    <cfRule type="cellIs" dxfId="29" priority="59" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="60" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91:C102">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C91)))</formula>
+  <conditionalFormatting sqref="C118:C129">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C118)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C91)))</formula>
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C118)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C136:C148">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C136)))</formula>
+  <conditionalFormatting sqref="C163:C175">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C136)))</formula>
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C137:C148">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  <conditionalFormatting sqref="C164:C175">
+    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C136:C148">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  <conditionalFormatting sqref="C163:C175">
+    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C136:C148">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+  <conditionalFormatting sqref="C163:C175">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C149)))</formula>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C149)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C176)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C149)))</formula>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C149)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C176)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C159">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="C176:C186">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C33:C39">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C98:C117">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C107:C117">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C107)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C107)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C136:C159 C2:C121">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C163:C186 C2:C148">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11263,7 +11728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -11404,8 +11869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13071,18 +13536,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C142">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:C123">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C101)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Auto loan Drawdown test case commit Stage: Disbursement maker stage User: Anandh
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="998">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2645,9 +2645,6 @@
     <t>AT_AL_DSB_DD_04</t>
   </si>
   <si>
-    <t>AT_AL_DSB_DD_05</t>
-  </si>
-  <si>
     <t>Payment_type</t>
   </si>
   <si>
@@ -3030,6 +3027,21 @@
   </si>
   <si>
     <t>mismatch</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_01</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_02</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_03</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_04</t>
+  </si>
+  <si>
+    <t>AT_AL_DSB_DDD_05</t>
   </si>
 </sst>
 </file>
@@ -3563,31 +3575,7 @@
     <cellStyle name="Result" xfId="7"/>
     <cellStyle name="Result2" xfId="8"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3729,210 +3717,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4489,16 +4273,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="37" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>306</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
   </sheetData>
@@ -7873,10 +7657,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C2" s="43">
         <v>4006</v>
@@ -8987,19 +8771,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>865</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>866</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>867</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>868</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>107</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -9016,7 +8800,7 @@
         <v>250</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>446</v>
@@ -9060,126 +8844,126 @@
         <v>318</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>889</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>891</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>892</v>
       </c>
       <c r="Z1" s="5" t="s">
         <v>28</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="AB1" s="5" t="s">
-        <v>894</v>
-      </c>
       <c r="AC1" s="83" t="s">
+        <v>989</v>
+      </c>
+      <c r="AD1" s="83" t="s">
         <v>990</v>
-      </c>
-      <c r="AD1" s="83" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="41" t="s">
+        <v>894</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>895</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>896</v>
       </c>
       <c r="C2" s="7">
         <v>5231</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>185</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>898</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>899</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>900</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>901</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>542</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>902</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>903</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>904</v>
       </c>
       <c r="N2" s="7">
         <v>987456</v>
@@ -9188,7 +8972,7 @@
         <v>974121</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Q2" s="7">
         <v>20</v>
@@ -9209,13 +8993,13 @@
         <v>250</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="X2" s="7">
         <v>10000</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
@@ -9223,51 +9007,51 @@
         <v>-123</v>
       </c>
       <c r="AC2" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="AD2" s="7" t="s">
         <v>992</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="41" t="s">
+        <v>907</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>908</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>909</v>
       </c>
       <c r="C3" s="7">
         <v>5231</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>185</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>898</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>899</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>900</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>901</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>542</v>
       </c>
       <c r="K3" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>902</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>903</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>904</v>
       </c>
       <c r="N3" s="7">
         <v>987456</v>
@@ -9276,7 +9060,7 @@
         <v>974121</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Q3" s="7">
         <v>20</v>
@@ -9297,28 +9081,28 @@
         <v>250</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="X3" s="7">
         <v>10000</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="Z3" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="AA3" s="7" t="s">
         <v>910</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>911</v>
       </c>
       <c r="AB3" s="7">
         <v>-123</v>
       </c>
       <c r="AC3" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="AD3" s="7" t="s">
         <v>992</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -9355,85 +9139,85 @@
         <v>318</v>
       </c>
       <c r="D1" s="78" t="s">
+        <v>925</v>
+      </c>
+      <c r="E1" s="78" t="s">
         <v>926</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="F1" s="78" t="s">
         <v>927</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="G1" s="78" t="s">
         <v>928</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="H1" s="78" t="s">
         <v>929</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="I1" s="78" t="s">
         <v>930</v>
       </c>
-      <c r="I1" s="78" t="s">
+      <c r="J1" s="78" t="s">
         <v>931</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="K1" s="78" t="s">
         <v>932</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="L1" s="78" t="s">
         <v>933</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="M1" s="78" t="s">
         <v>934</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="N1" s="78" t="s">
         <v>935</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="O1" s="78" t="s">
         <v>936</v>
       </c>
-      <c r="O1" s="78" t="s">
+      <c r="P1" s="78" t="s">
         <v>937</v>
       </c>
-      <c r="P1" s="78" t="s">
+      <c r="Q1" s="78" t="s">
         <v>938</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="R1" s="78" t="s">
         <v>939</v>
       </c>
-      <c r="R1" s="78" t="s">
+      <c r="S1" s="78" t="s">
         <v>940</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="T1" s="78" t="s">
         <v>941</v>
-      </c>
-      <c r="T1" s="78" t="s">
-        <v>942</v>
       </c>
       <c r="U1" s="78" t="s">
         <v>125</v>
       </c>
       <c r="V1" s="78" t="s">
+        <v>942</v>
+      </c>
+      <c r="W1" s="78" t="s">
         <v>943</v>
       </c>
-      <c r="W1" s="78" t="s">
+      <c r="X1" s="78" t="s">
         <v>944</v>
       </c>
-      <c r="X1" s="78" t="s">
+      <c r="Y1" s="78" t="s">
         <v>945</v>
       </c>
-      <c r="Y1" s="78" t="s">
+      <c r="Z1" s="78" t="s">
         <v>946</v>
       </c>
-      <c r="Z1" s="78" t="s">
+      <c r="AA1" s="78" t="s">
         <v>947</v>
       </c>
-      <c r="AA1" s="78" t="s">
+      <c r="AB1" s="78" t="s">
         <v>948</v>
       </c>
-      <c r="AB1" s="78" t="s">
+      <c r="AC1" s="78" t="s">
         <v>949</v>
       </c>
-      <c r="AC1" s="78" t="s">
+      <c r="AD1" s="78" t="s">
         <v>950</v>
-      </c>
-      <c r="AD1" s="78" t="s">
-        <v>951</v>
       </c>
       <c r="AE1" s="78" t="s">
         <v>62</v>
@@ -9445,39 +9229,39 @@
         <v>154</v>
       </c>
       <c r="AH1" s="78" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.75">
       <c r="A2" s="79" t="s">
+        <v>952</v>
+      </c>
+      <c r="B2" s="79" t="s">
         <v>953</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>954</v>
       </c>
       <c r="C2">
         <v>4138</v>
       </c>
       <c r="D2" s="79" t="s">
+        <v>954</v>
+      </c>
+      <c r="E2" s="79" t="s">
         <v>955</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>956</v>
-      </c>
-      <c r="F2" s="78" t="s">
-        <v>957</v>
       </c>
       <c r="G2" s="81">
         <v>36779</v>
       </c>
       <c r="H2" s="78" t="s">
+        <v>957</v>
+      </c>
+      <c r="I2" s="78" t="s">
         <v>958</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="J2" s="78" t="s">
         <v>959</v>
-      </c>
-      <c r="J2" s="78" t="s">
-        <v>960</v>
       </c>
       <c r="K2" s="78" t="s">
         <v>82</v>
@@ -9489,28 +9273,28 @@
         <v>217</v>
       </c>
       <c r="N2" s="78" t="s">
+        <v>960</v>
+      </c>
+      <c r="O2" s="78" t="s">
         <v>961</v>
       </c>
-      <c r="O2" s="78" t="s">
+      <c r="P2" s="78" t="s">
         <v>962</v>
       </c>
-      <c r="P2" s="78" t="s">
+      <c r="Q2" s="78" t="s">
         <v>963</v>
-      </c>
-      <c r="Q2" s="78" t="s">
-        <v>964</v>
       </c>
       <c r="R2" s="78" t="s">
         <v>384</v>
       </c>
       <c r="S2" s="78" t="s">
+        <v>964</v>
+      </c>
+      <c r="T2" s="82" t="s">
         <v>965</v>
       </c>
-      <c r="T2" s="82" t="s">
+      <c r="U2" s="78" t="s">
         <v>966</v>
-      </c>
-      <c r="U2" s="78" t="s">
-        <v>967</v>
       </c>
       <c r="V2" s="78" t="s">
         <v>156</v>
@@ -9519,25 +9303,25 @@
         <v>156</v>
       </c>
       <c r="X2" s="78" t="s">
+        <v>967</v>
+      </c>
+      <c r="Y2" s="78" t="s">
+        <v>967</v>
+      </c>
+      <c r="Z2" s="78" t="s">
         <v>968</v>
-      </c>
-      <c r="Y2" s="78" t="s">
-        <v>968</v>
-      </c>
-      <c r="Z2" s="78" t="s">
-        <v>969</v>
       </c>
       <c r="AA2" s="78" t="s">
         <v>542</v>
       </c>
       <c r="AB2" s="78" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AC2" s="78" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AD2" s="78" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AE2" s="78" t="s">
         <v>74</v>
@@ -9546,10 +9330,10 @@
         <v>31</v>
       </c>
       <c r="AG2" s="78" t="s">
+        <v>970</v>
+      </c>
+      <c r="AH2" s="78" t="s">
         <v>971</v>
-      </c>
-      <c r="AH2" s="78" t="s">
-        <v>972</v>
       </c>
     </row>
   </sheetData>
@@ -9566,10 +9350,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10116,10 +9900,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="80" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B48" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>24</v>
@@ -10127,10 +9911,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="80" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B49" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>24</v>
@@ -10138,10 +9922,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="80" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B50" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>24</v>
@@ -10149,10 +9933,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="80" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B51" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>24</v>
@@ -10160,10 +9944,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="80" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B52" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>24</v>
@@ -10171,10 +9955,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="80" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B53" s="80" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>24</v>
@@ -11218,7 +11002,7 @@
         <v>294</v>
       </c>
       <c r="B149" s="18"/>
-      <c r="C149" s="35" t="s">
+      <c r="C149" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11229,7 +11013,7 @@
       <c r="B150" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="C150" s="35" t="s">
+      <c r="C150" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11240,7 +11024,7 @@
       <c r="B151" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C151" s="68" t="s">
+      <c r="C151" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11251,7 +11035,7 @@
       <c r="B152" s="20" t="s">
         <v>746</v>
       </c>
-      <c r="C152" s="35" t="s">
+      <c r="C152" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11262,7 +11046,7 @@
       <c r="B153" s="20" t="s">
         <v>753</v>
       </c>
-      <c r="C153" s="35" t="s">
+      <c r="C153" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11273,7 +11057,7 @@
       <c r="B154" s="20" t="s">
         <v>762</v>
       </c>
-      <c r="C154" s="35" t="s">
+      <c r="C154" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11282,7 +11066,7 @@
         <v>857</v>
       </c>
       <c r="B155" s="18"/>
-      <c r="C155" s="35" t="s">
+      <c r="C155" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11293,7 +11077,7 @@
       <c r="B156" s="20" t="s">
         <v>859</v>
       </c>
-      <c r="C156" s="35" t="s">
+      <c r="C156" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11302,105 +11086,97 @@
         <v>860</v>
       </c>
       <c r="B157" s="18"/>
-      <c r="C157" s="35" t="s">
+      <c r="C157" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="22" t="s">
-        <v>861</v>
+        <v>993</v>
       </c>
       <c r="B158" s="18"/>
-      <c r="C158" s="35" t="s">
+      <c r="C158" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="22" t="s">
-        <v>862</v>
+        <v>994</v>
       </c>
       <c r="B159" s="18"/>
-      <c r="C159" s="35" t="s">
+      <c r="C159" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="22" t="s">
-        <v>863</v>
+        <v>995</v>
       </c>
       <c r="B160" s="18"/>
-      <c r="C160" s="35" t="s">
+      <c r="C160" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="22" t="s">
-        <v>864</v>
+        <v>996</v>
       </c>
       <c r="B161" s="18"/>
-      <c r="C161" s="35" t="s">
+      <c r="C161" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="22" t="s">
-        <v>865</v>
+        <v>997</v>
       </c>
       <c r="B162" s="18"/>
-      <c r="C162" s="35" t="s">
+      <c r="C162" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" s="80" t="s">
-        <v>895</v>
-      </c>
-      <c r="B163" s="80" t="s">
-        <v>896</v>
-      </c>
+      <c r="A163" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="B163" s="18"/>
       <c r="C163" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="80" t="s">
-        <v>912</v>
-      </c>
-      <c r="B164" s="80" t="s">
-        <v>896</v>
-      </c>
+      <c r="A164" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="B164" s="18"/>
       <c r="C164" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="80" t="s">
-        <v>913</v>
-      </c>
-      <c r="B165" s="80" t="s">
-        <v>896</v>
-      </c>
+      <c r="A165" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="B165" s="18"/>
       <c r="C165" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="80" t="s">
-        <v>914</v>
-      </c>
-      <c r="B166" s="80" t="s">
-        <v>896</v>
-      </c>
+      <c r="A166" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="B166" s="18"/>
       <c r="C166" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="80" t="s">
-        <v>915</v>
+        <v>894</v>
       </c>
       <c r="B167" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C167" s="20" t="s">
         <v>24</v>
@@ -11408,10 +11184,10 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="80" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="B168" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C168" s="20" t="s">
         <v>24</v>
@@ -11419,10 +11195,10 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="80" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="B169" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C169" s="20" t="s">
         <v>24</v>
@@ -11430,10 +11206,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="80" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="B170" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C170" s="20" t="s">
         <v>24</v>
@@ -11441,10 +11217,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="80" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="B171" s="80" t="s">
-        <v>909</v>
+        <v>895</v>
       </c>
       <c r="C171" s="20" t="s">
         <v>24</v>
@@ -11452,10 +11228,10 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="80" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="B172" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C172" s="20" t="s">
         <v>24</v>
@@ -11463,10 +11239,10 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="80" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="B173" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C173" s="20" t="s">
         <v>24</v>
@@ -11474,10 +11250,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="80" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="B174" s="80" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C174" s="20" t="s">
         <v>24</v>
@@ -11485,10 +11261,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="80" t="s">
-        <v>922</v>
+        <v>907</v>
       </c>
       <c r="B175" s="80" t="s">
-        <v>896</v>
+        <v>908</v>
       </c>
       <c r="C175" s="20" t="s">
         <v>24</v>
@@ -11496,10 +11272,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="80" t="s">
-        <v>953</v>
+        <v>918</v>
       </c>
       <c r="B176" s="80" t="s">
-        <v>954</v>
+        <v>895</v>
       </c>
       <c r="C176" s="20" t="s">
         <v>24</v>
@@ -11507,10 +11283,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="80" t="s">
-        <v>973</v>
+        <v>919</v>
       </c>
       <c r="B177" s="80" t="s">
-        <v>954</v>
+        <v>895</v>
       </c>
       <c r="C177" s="20" t="s">
         <v>24</v>
@@ -11518,10 +11294,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="80" t="s">
-        <v>974</v>
+        <v>920</v>
       </c>
       <c r="B178" s="80" t="s">
-        <v>954</v>
+        <v>895</v>
       </c>
       <c r="C178" s="20" t="s">
         <v>24</v>
@@ -11529,10 +11305,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="80" t="s">
-        <v>975</v>
+        <v>921</v>
       </c>
       <c r="B179" s="80" t="s">
-        <v>954</v>
+        <v>895</v>
       </c>
       <c r="C179" s="20" t="s">
         <v>24</v>
@@ -11540,10 +11316,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="80" t="s">
-        <v>976</v>
+        <v>952</v>
       </c>
       <c r="B180" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C180" s="20" t="s">
         <v>24</v>
@@ -11551,10 +11327,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="80" t="s">
-        <v>977</v>
+        <v>972</v>
       </c>
       <c r="B181" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C181" s="20" t="s">
         <v>24</v>
@@ -11562,10 +11338,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="80" t="s">
-        <v>978</v>
+        <v>973</v>
       </c>
       <c r="B182" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C182" s="20" t="s">
         <v>24</v>
@@ -11573,10 +11349,10 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="80" t="s">
-        <v>979</v>
+        <v>974</v>
       </c>
       <c r="B183" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C183" s="20" t="s">
         <v>24</v>
@@ -11584,10 +11360,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="80" t="s">
-        <v>980</v>
+        <v>975</v>
       </c>
       <c r="B184" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C184" s="20" t="s">
         <v>24</v>
@@ -11595,10 +11371,10 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="80" t="s">
-        <v>981</v>
+        <v>976</v>
       </c>
       <c r="B185" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C185" s="20" t="s">
         <v>24</v>
@@ -11606,116 +11382,86 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="80" t="s">
-        <v>982</v>
+        <v>977</v>
       </c>
       <c r="B186" s="80" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C186" s="20" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="80" t="s">
+        <v>978</v>
+      </c>
+      <c r="B187" s="80" t="s">
+        <v>953</v>
+      </c>
+      <c r="C187" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="80" t="s">
+        <v>979</v>
+      </c>
+      <c r="B188" s="80" t="s">
+        <v>953</v>
+      </c>
+      <c r="C188" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="80" t="s">
+        <v>980</v>
+      </c>
+      <c r="B189" s="80" t="s">
+        <v>953</v>
+      </c>
+      <c r="C189" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="80" t="s">
+        <v>981</v>
+      </c>
+      <c r="B190" s="80" t="s">
+        <v>953</v>
+      </c>
+      <c r="C190" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C148">
-    <cfRule type="cellIs" dxfId="29" priority="59" operator="equal">
+  <conditionalFormatting sqref="C2:C166">
+    <cfRule type="cellIs" dxfId="16" priority="61" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C118:C129">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C118)))</formula>
+  <conditionalFormatting sqref="C107:C129">
+    <cfRule type="containsText" dxfId="14" priority="29" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C118)))</formula>
+    <cfRule type="containsText" dxfId="13" priority="30" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C163:C175">
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C163)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C163)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C164:C175">
-    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C163:C175">
-    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C163:C175">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+  <conditionalFormatting sqref="C167:C190">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C176)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C176)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C176)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C176)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C176:C186">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C39">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98:C117">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C107:C117">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",C107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C107)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C163:C186 C2:C148">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C190">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13536,18 +13282,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C142">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:C123">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C101)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Application details new app changed test case committed
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
+++ b/AzentioAutomationFramework_AutoLoan/TestData/ULS_AutoLoanTestData.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="999">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -3042,6 +3042,9 @@
   </si>
   <si>
     <t>AT_AL_DSB_DDD_05</t>
+  </si>
+  <si>
+    <t>5571</t>
   </si>
 </sst>
 </file>
@@ -4078,11 +4081,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
+    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4316,14 +4319,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="25.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4403,31 +4406,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" style="44" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="44" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -5024,25 +5027,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5442,15 +5445,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="44" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="44" width="25.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5610,20 +5613,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5837,9 +5840,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5879,17 +5882,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
@@ -5978,26 +5981,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -6139,37 +6142,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="9" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="9" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.42578125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="48.75" customHeight="1">
@@ -6386,16 +6389,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6616,38 +6619,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="31.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="31.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="24" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="31.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="26.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.859375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="30.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="32.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="43.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="30.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="28.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="4" width="32.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="21.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="40.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="4" width="31.140625" collapsed="true"/>
+    <col min="21" max="23" customWidth="true" style="4" width="31.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="4" width="19.42578125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="24.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="4" width="19.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="4" width="17.5703125" collapsed="true"/>
+    <col min="34" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6907,7 +6910,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>855</v>
+        <v>998</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -7013,28 +7016,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -7402,17 +7405,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7631,11 +7634,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7737,8 +7740,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7778,11 +7781,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7851,11 +7854,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7924,11 +7927,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7997,9 +8000,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8039,29 +8042,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -8284,16 +8287,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="4" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="17.42578125" collapsed="true"/>
+    <col min="8" max="8" style="4" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="13.7109375" collapsed="true"/>
+    <col min="10" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -8369,16 +8372,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="29.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="45" width="41.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="21.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="16.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="49" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="24.5703125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="4" width="29.7109375" collapsed="true"/>
+    <col min="7" max="45" customWidth="true" style="4" width="41.42578125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="4" width="21.85546875" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="4" width="16.5703125" collapsed="true"/>
+    <col min="49" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -8755,12 +8758,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -8824,13 +8827,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="28" max="28" width="20.7109375" customWidth="1"/>
-    <col min="30" max="30" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -9123,9 +9126,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75">
@@ -9358,14 +9361,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -11480,13 +11483,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -11621,9 +11624,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -13316,24 +13319,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="40.140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="39.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20" style="4" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="29.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="4" width="40.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="22.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="23.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="4" width="39.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="4" width="23.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="4" width="20.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="4" width="18.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="4" width="20.0" collapsed="true"/>
+    <col min="19" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -13542,28 +13545,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -13774,23 +13777,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -14016,28 +14019,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -14260,11 +14263,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14360,9 +14363,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>